<commit_message>
dynamic coupling of metabolism
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -2105,10 +2105,10 @@
   <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2194,7 +2194,7 @@
         <v>253</v>
       </c>
       <c r="B6" s="2">
-        <v>1E-4</v>
+        <v>8.3329999999999997E-6</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>249</v>
@@ -2306,7 +2306,7 @@
         <v>261</v>
       </c>
       <c r="B14" s="2">
-        <v>1E-4</v>
+        <v>8.3329999999999997E-6</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>249</v>
@@ -2334,7 +2334,7 @@
         <v>263</v>
       </c>
       <c r="B16" s="2">
-        <v>1E-4</v>
+        <v>8.3329999999999997E-6</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>249</v>
@@ -2362,7 +2362,7 @@
         <v>265</v>
       </c>
       <c r="B18" s="2">
-        <v>1E-4</v>
+        <v>8.3329999999999997E-6</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>249</v>
@@ -2530,7 +2530,7 @@
         <v>277</v>
       </c>
       <c r="B30" s="2">
-        <v>1E-4</v>
+        <v>8.3329999999999997E-6</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>249</v>
@@ -2558,7 +2558,7 @@
         <v>279</v>
       </c>
       <c r="B32" s="2">
-        <v>1E-4</v>
+        <v>8.3329999999999997E-6</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>249</v>
@@ -3524,7 +3524,7 @@
         <v>348</v>
       </c>
       <c r="B101" s="2">
-        <v>1E-4</v>
+        <v>8.3329999999999997E-6</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>249</v>
@@ -3552,7 +3552,7 @@
         <v>350</v>
       </c>
       <c r="B103" s="2">
-        <v>1E-4</v>
+        <v>8.3329999999999997E-6</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
Change complex subunits to species types
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="555" windowWidth="27495" windowHeight="11445" tabRatio="865" activeTab="11"/>
+    <workbookView xWindow="636" yWindow="552" windowWidth="27492" windowHeight="11448" tabRatio="865" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="393">
   <si>
     <t>Id</t>
   </si>
@@ -781,9 +781,6 @@
   </si>
   <si>
     <t>process_RibosomeAssembly</t>
-  </si>
-  <si>
-    <t>[c]: prot_gene_1_2</t>
   </si>
   <si>
     <t>Species</t>
@@ -1592,7 +1589,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -1675,7 +1672,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -2035,10 +2032,10 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -2084,7 +2081,7 @@
         <v>243</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2104,24 +2101,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
@@ -2135,13 +2132,13 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B2" s="2">
         <v>1E-4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2149,13 +2146,13 @@
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B3" s="2">
         <v>2E-3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2163,13 +2160,13 @@
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B4" s="2">
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2177,13 +2174,13 @@
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B5" s="2">
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2191,13 +2188,13 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2205,13 +2202,13 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B7" s="2">
         <v>2E-3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2219,13 +2216,13 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B8" s="2">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2233,13 +2230,13 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B9" s="2">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2247,13 +2244,13 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B10" s="2">
         <v>5.1000000000000004E-4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2261,13 +2258,13 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B11" s="2">
         <v>5.1000000000000004E-4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2275,13 +2272,13 @@
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B12" s="2">
         <v>4.1999999999999997E-3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2289,13 +2286,13 @@
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B13" s="2">
         <v>4.1999999999999997E-3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2303,13 +2300,13 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B14" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2317,13 +2314,13 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B15" s="2">
         <v>2E-3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2331,13 +2328,13 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B16" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2345,13 +2342,13 @@
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B17" s="2">
         <v>2E-3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2359,13 +2356,13 @@
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B18" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -2373,13 +2370,13 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B19" s="2">
         <v>2E-3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -2387,13 +2384,13 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B20" s="2">
         <v>3.6999999999999999E-4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2401,13 +2398,13 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B21" s="2">
         <v>3.6999999999999999E-4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -2415,13 +2412,13 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B22" s="2">
         <v>1E-4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -2429,13 +2426,13 @@
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B23" s="2">
         <v>2E-3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2443,13 +2440,13 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B24" s="2">
         <v>3.8E-3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2457,13 +2454,13 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B25" s="2">
         <v>3.8E-3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2471,13 +2468,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B26" s="2">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2485,13 +2482,13 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B27" s="2">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2499,13 +2496,13 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B28" s="2">
         <v>3.0999999999999999E-3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2513,13 +2510,13 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B29" s="2">
         <v>3.0999999999999999E-3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2527,13 +2524,13 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B30" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2541,13 +2538,13 @@
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B31" s="2">
         <v>2E-3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -2555,13 +2552,13 @@
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B32" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2569,13 +2566,13 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B33" s="2">
         <v>2E-3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2583,13 +2580,13 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B34" s="2">
         <v>0.5</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2597,13 +2594,13 @@
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B35" s="2">
         <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2611,13 +2608,13 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B36" s="2">
         <v>1E-4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2625,13 +2622,13 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B37" s="2">
         <v>2E-3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2639,13 +2636,13 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B38" s="2">
         <v>6.7999999999999999E-5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2653,13 +2650,13 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B39" s="2">
         <v>6.7999999999999999E-5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2667,13 +2664,13 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B40" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2681,13 +2678,13 @@
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B41" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2695,13 +2692,13 @@
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B42" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2709,13 +2706,13 @@
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B43" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2723,13 +2720,13 @@
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B44" s="2">
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2737,13 +2734,13 @@
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B45" s="2">
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2751,13 +2748,13 @@
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B46" s="2">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2765,13 +2762,13 @@
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B47" s="2">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2779,13 +2776,13 @@
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B48" s="2">
         <v>1.8E-5</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2793,13 +2790,13 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B49" s="2">
         <v>1.8E-5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2807,13 +2804,13 @@
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B50" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2821,13 +2818,13 @@
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B51" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2835,13 +2832,13 @@
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B52" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -2849,13 +2846,13 @@
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B53" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -2863,13 +2860,13 @@
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B54" s="2">
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2877,13 +2874,13 @@
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B55" s="2">
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2891,13 +2888,13 @@
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B56" s="2">
         <v>1.8431983348741521E-7</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2905,13 +2902,13 @@
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B57" s="2">
         <v>1.5276959171929909E-7</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2919,13 +2916,13 @@
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B58" s="2">
         <v>1.4446689651716331E-7</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -2933,13 +2930,13 @@
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B59" s="2">
         <v>1.8099875540656089E-7</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -2947,13 +2944,13 @@
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B60" s="2">
         <v>1.5941174788100771E-7</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -2961,13 +2958,13 @@
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B61" s="2">
         <v>1.8099875540656089E-7</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -2975,13 +2972,13 @@
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B62" s="2">
         <v>1.5609066980015339E-7</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -2989,13 +2986,13 @@
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B63" s="2">
         <v>1.793382163661337E-7</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -3003,13 +3000,13 @@
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B64" s="2">
         <v>1.793382163661337E-7</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -3017,13 +3014,13 @@
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B65" s="2">
         <v>1.7269606020442511E-7</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -3031,13 +3028,13 @@
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B66" s="2">
         <v>1.1789827187032859E-7</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -3045,13 +3042,13 @@
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B67" s="2">
         <v>1.9262252868955099E-7</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -3059,13 +3056,13 @@
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B68" s="2">
         <v>2.042463019725412E-7</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -3073,13 +3070,13 @@
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B69" s="2">
         <v>1.8431983348741521E-7</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -3087,13 +3084,13 @@
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B70" s="2">
         <v>0.01</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -3101,13 +3098,13 @@
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B71" s="2">
         <v>1.4778797459801761E-7</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -3115,13 +3112,13 @@
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B72" s="2">
         <v>0.01</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -3129,13 +3126,13 @@
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B73" s="2">
         <v>1.7767767732570659E-7</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -3143,13 +3140,13 @@
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B74" s="2">
         <v>0.01</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -3157,13 +3154,13 @@
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B75" s="2">
         <v>1.4114581843630891E-7</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -3171,13 +3168,13 @@
     </row>
     <row r="76" spans="1:6" ht="15" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B76" s="2">
         <v>0.01</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -3185,13 +3182,13 @@
     </row>
     <row r="77" spans="1:6" ht="15" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B77" s="2">
         <v>1.7103552116399789E-7</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -3199,13 +3196,13 @@
     </row>
     <row r="78" spans="1:6" ht="15" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B78" s="2">
         <v>0.01</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -3213,13 +3210,13 @@
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B79" s="2">
         <v>1.6273282596186211E-7</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -3227,13 +3224,13 @@
     </row>
     <row r="80" spans="1:6" ht="15" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B80" s="2">
         <v>0.01</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -3241,13 +3238,13 @@
     </row>
     <row r="81" spans="1:6" ht="15" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B81" s="2">
         <v>2.042463019725412E-7</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -3255,13 +3252,13 @@
     </row>
     <row r="82" spans="1:6" ht="15" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B82" s="2">
         <v>0.01</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -3269,13 +3266,13 @@
     </row>
     <row r="83" spans="1:6" ht="15" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B83" s="2">
         <v>1.5443013075972631E-7</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -3283,13 +3280,13 @@
     </row>
     <row r="84" spans="1:6" ht="15" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B84" s="2">
         <v>0.01</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -3297,13 +3294,13 @@
     </row>
     <row r="85" spans="1:6" ht="15" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B85" s="2">
         <v>1.2454042803203729E-7</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -3311,13 +3308,13 @@
     </row>
     <row r="86" spans="1:6" ht="15" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B86" s="2">
         <v>0.01</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -3325,13 +3322,13 @@
     </row>
     <row r="87" spans="1:6" ht="15" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B87" s="2">
         <v>1.9262252868955099E-7</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -3339,13 +3336,13 @@
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B88" s="2">
         <v>0.01</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -3353,13 +3350,13 @@
     </row>
     <row r="89" spans="1:6" ht="15" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B89" s="2">
         <v>1.428063574767361E-7</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -3367,13 +3364,13 @@
     </row>
     <row r="90" spans="1:6" ht="15" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B90" s="2">
         <v>0.01</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -3381,13 +3378,13 @@
     </row>
     <row r="91" spans="1:6" ht="15" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B91" s="2">
         <v>1.3450366227460029E-7</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -3395,13 +3392,13 @@
     </row>
     <row r="92" spans="1:6" ht="15" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B92" s="2">
         <v>0.01</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -3409,13 +3406,13 @@
     </row>
     <row r="93" spans="1:6" ht="15" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B93" s="2">
         <v>6.7999999999999999E-5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -3423,13 +3420,13 @@
     </row>
     <row r="94" spans="1:6" ht="15" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B94" s="2">
         <v>6.7999999999999999E-5</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -3437,13 +3434,13 @@
     </row>
     <row r="95" spans="1:6" ht="15" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B95" s="2">
         <v>1.8000000000000001E-4</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -3451,13 +3448,13 @@
     </row>
     <row r="96" spans="1:6" ht="15" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B96" s="2">
         <v>1.8000000000000001E-4</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -3465,13 +3462,13 @@
     </row>
     <row r="97" spans="1:6" ht="15" customHeight="1">
       <c r="A97" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B97" s="2">
         <v>1.2E-5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -3479,13 +3476,13 @@
     </row>
     <row r="98" spans="1:6" ht="15" customHeight="1">
       <c r="A98" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B98" s="2">
         <v>1.2E-5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -3493,13 +3490,13 @@
     </row>
     <row r="99" spans="1:6" ht="15" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B99" s="2">
         <v>2.9E-5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -3507,13 +3504,13 @@
     </row>
     <row r="100" spans="1:6" ht="15" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B100" s="2">
         <v>2.9E-5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -3521,13 +3518,13 @@
     </row>
     <row r="101" spans="1:6" ht="15" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B101" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -3535,13 +3532,13 @@
     </row>
     <row r="102" spans="1:6" ht="15" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B102" s="2">
         <v>2E-3</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -3549,13 +3546,13 @@
     </row>
     <row r="103" spans="1:6" ht="15" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B103" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -3563,13 +3560,13 @@
     </row>
     <row r="104" spans="1:6" ht="15" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B104" s="2">
         <v>2E-3</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -3577,13 +3574,13 @@
     </row>
     <row r="105" spans="1:6" ht="15" customHeight="1">
       <c r="A105" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B105" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -3591,13 +3588,13 @@
     </row>
     <row r="106" spans="1:6" ht="15" customHeight="1">
       <c r="A106" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B106" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -3613,14 +3610,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -3630,13 +3627,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -3665,23 +3662,23 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -3710,7 +3707,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -3720,10 +3717,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>11</v>
@@ -3737,14 +3734,14 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
         <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3752,14 +3749,14 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
         <v>1000000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -3767,14 +3764,14 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
         <v>0.3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -3782,14 +3779,14 @@
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
         <v>1.0000000000000001E-15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3812,7 +3809,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -3822,13 +3819,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -3842,16 +3839,16 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>373</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3860,16 +3857,16 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>375</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -3878,7 +3875,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>242</v>
@@ -3887,7 +3884,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -3896,16 +3893,16 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>378</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3914,16 +3911,16 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -3932,16 +3929,16 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>382</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -3950,16 +3947,16 @@
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -3968,16 +3965,16 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -3986,16 +3983,16 @@
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -4004,16 +4001,16 @@
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4022,16 +4019,16 @@
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -4055,14 +4052,14 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -4082,7 +4079,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4127,7 +4124,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4190,7 +4187,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4742,7 +4739,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4809,7 +4806,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4863,7 +4860,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -5241,7 +5238,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -5604,7 +5601,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Add string attribute to store subunit composition in uniprot ids
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="636" yWindow="552" windowWidth="27492" windowHeight="11448" tabRatio="865" firstSheet="3" activeTab="12"/>
+    <workbookView xWindow="636" yWindow="552" windowWidth="27492" windowHeight="11448" tabRatio="865" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cell!$A$1:$B$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Compartments!$A$1:$F$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Complex species types'!$A$1:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Complex species types'!$A$1:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Concentrations!$A$1:$F$106</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'DNA species types'!$A$1:$I$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Gene loci'!$A$1:$K$17</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="394">
   <si>
     <t>Id</t>
   </si>
@@ -1228,6 +1228,9 @@
   </si>
   <si>
     <t>Standard id</t>
+  </si>
+  <si>
+    <t>Composition in Uniprot</t>
   </si>
 </sst>
 </file>
@@ -2026,18 +2029,18 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1">
+    <row r="1" spans="1:12" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2051,28 +2054,31 @@
         <v>238</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1">
+    <row r="2" spans="1:12" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>242</v>
       </c>
@@ -2090,9 +2096,10 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K2"/>
+  <autoFilter ref="A1:L2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3610,7 +3617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
Add ploidy attribute to DNA species type
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="555" windowWidth="27495" windowHeight="11445" tabRatio="865" firstSheet="6" activeTab="14"/>
+    <workbookView xWindow="630" yWindow="555" windowWidth="20730" windowHeight="11445" tabRatio="865" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Compartments!$A$1:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Complex species types'!$A$1:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Concentrations!$A$1:$F$106</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'DNA species types'!$A$1:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'DNA species types'!$A$1:$J$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Gene loci'!$A$1:$K$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Knowledge base'!$A$1:$B$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Metabolite species types'!$A$1:$G$35</definedName>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="397">
   <si>
     <t>Id</t>
   </si>
@@ -1238,6 +1238,9 @@
   </si>
   <si>
     <t>Database References</t>
+  </si>
+  <si>
+    <t>Ploidy</t>
   </si>
 </sst>
 </file>
@@ -3740,7 +3743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -4811,18 +4814,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1">
+    <row r="1" spans="1:10" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4839,19 +4842,22 @@
         <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:10" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>125</v>
       </c>
@@ -4865,13 +4871,16 @@
       <c r="E2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I2"/>
+  <autoFilter ref="A1:J2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Change excel files due to changing sequence attribute of DnaSpeciesType to sequence_path attribute
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="555" windowWidth="20730" windowHeight="11445" tabRatio="865" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="636" yWindow="552" windowWidth="20736" windowHeight="11448" tabRatio="865" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -418,9 +418,6 @@
     <t>InChI=1S/C5H11NO2/c1-3(2)4(6)5(7)8/h3-4H,6H2,1-2H3,(H,7,8)/t4-/m0/s1</t>
   </si>
   <si>
-    <t>Sequence</t>
-  </si>
-  <si>
     <t>Circular</t>
   </si>
   <si>
@@ -1241,6 +1238,9 @@
   </si>
   <si>
     <t>Ploidy</t>
+  </si>
+  <si>
+    <t>Sequence Path</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1628,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -1711,7 +1711,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -1721,16 +1721,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>22</v>
@@ -1747,16 +1747,16 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>0</v>
@@ -1773,16 +1773,16 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>0</v>
@@ -1799,16 +1799,16 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E4" s="2" t="b">
         <v>0</v>
@@ -1825,16 +1825,16 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E5" s="2" t="b">
         <v>0</v>
@@ -1851,16 +1851,16 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E6" s="2" t="b">
         <v>0</v>
@@ -1877,16 +1877,16 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>0</v>
@@ -1903,16 +1903,16 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>0</v>
@@ -1929,16 +1929,16 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
@@ -1955,16 +1955,16 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>0</v>
@@ -1981,16 +1981,16 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
@@ -2007,16 +2007,16 @@
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
@@ -2033,16 +2033,16 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
@@ -2074,7 +2074,7 @@
       <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -2084,22 +2084,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>22</v>
@@ -2116,14 +2116,14 @@
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2151,17 +2151,17 @@
       <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="2">
         <v>1E-4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2189,13 +2189,13 @@
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B3" s="2">
         <v>2E-3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2203,13 +2203,13 @@
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B4" s="2">
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2217,13 +2217,13 @@
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B5" s="2">
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2231,13 +2231,13 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B7" s="2">
         <v>2E-3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B8" s="2">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2273,13 +2273,13 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B9" s="2">
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2287,13 +2287,13 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B10" s="2">
         <v>5.1000000000000004E-4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2301,13 +2301,13 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B11" s="2">
         <v>5.1000000000000004E-4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2315,13 +2315,13 @@
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B12" s="2">
         <v>4.1999999999999997E-3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2329,13 +2329,13 @@
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B13" s="2">
         <v>4.1999999999999997E-3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -2343,13 +2343,13 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B14" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -2357,13 +2357,13 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B15" s="2">
         <v>2E-3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2371,13 +2371,13 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B16" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2385,13 +2385,13 @@
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B17" s="2">
         <v>2E-3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2399,13 +2399,13 @@
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B18" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -2413,13 +2413,13 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B19" s="2">
         <v>2E-3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -2427,13 +2427,13 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B20" s="2">
         <v>3.6999999999999999E-4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2441,13 +2441,13 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B21" s="2">
         <v>3.6999999999999999E-4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -2455,13 +2455,13 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B22" s="2">
         <v>1E-4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -2469,13 +2469,13 @@
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B23" s="2">
         <v>2E-3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2483,13 +2483,13 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B24" s="2">
         <v>3.8E-3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2497,13 +2497,13 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B25" s="2">
         <v>3.8E-3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2511,13 +2511,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B26" s="2">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2525,13 +2525,13 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B27" s="2">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B28" s="2">
         <v>3.0999999999999999E-3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2553,13 +2553,13 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B29" s="2">
         <v>3.0999999999999999E-3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2567,13 +2567,13 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B30" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2581,13 +2581,13 @@
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B31" s="2">
         <v>2E-3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -2595,13 +2595,13 @@
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B32" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2609,13 +2609,13 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B33" s="2">
         <v>2E-3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2623,13 +2623,13 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B34" s="2">
         <v>0.5</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2637,13 +2637,13 @@
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B35" s="2">
         <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2651,13 +2651,13 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B36" s="2">
         <v>1E-4</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2665,13 +2665,13 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B37" s="2">
         <v>2E-3</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2679,13 +2679,13 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B38" s="2">
         <v>6.7999999999999999E-5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2693,13 +2693,13 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B39" s="2">
         <v>6.7999999999999999E-5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2707,13 +2707,13 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B40" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2721,13 +2721,13 @@
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B41" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2735,13 +2735,13 @@
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B42" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2749,13 +2749,13 @@
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B43" s="2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2763,13 +2763,13 @@
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B44" s="2">
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2777,13 +2777,13 @@
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B45" s="2">
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2791,13 +2791,13 @@
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B46" s="2">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2805,13 +2805,13 @@
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B47" s="2">
         <v>1.4999999999999999E-4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2819,13 +2819,13 @@
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B48" s="2">
         <v>1.8E-5</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2833,13 +2833,13 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B49" s="2">
         <v>1.8E-5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2847,13 +2847,13 @@
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B50" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2861,13 +2861,13 @@
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B51" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2875,13 +2875,13 @@
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B52" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -2889,13 +2889,13 @@
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B53" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -2903,13 +2903,13 @@
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B54" s="2">
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2917,13 +2917,13 @@
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B55" s="2">
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2931,13 +2931,13 @@
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B56" s="2">
         <v>1.8431983348741521E-7</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2945,13 +2945,13 @@
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B57" s="2">
         <v>1.5276959171929909E-7</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2959,13 +2959,13 @@
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B58" s="2">
         <v>1.4446689651716331E-7</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -2973,13 +2973,13 @@
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B59" s="2">
         <v>1.8099875540656089E-7</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -2987,13 +2987,13 @@
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B60" s="2">
         <v>1.5941174788100771E-7</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -3001,13 +3001,13 @@
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B61" s="2">
         <v>1.8099875540656089E-7</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -3015,13 +3015,13 @@
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B62" s="2">
         <v>1.5609066980015339E-7</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -3029,13 +3029,13 @@
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B63" s="2">
         <v>1.793382163661337E-7</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -3043,13 +3043,13 @@
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B64" s="2">
         <v>1.793382163661337E-7</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -3057,13 +3057,13 @@
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B65" s="2">
         <v>1.7269606020442511E-7</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -3071,13 +3071,13 @@
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B66" s="2">
         <v>1.1789827187032859E-7</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -3085,13 +3085,13 @@
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B67" s="2">
         <v>1.9262252868955099E-7</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -3099,13 +3099,13 @@
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B68" s="2">
         <v>2.042463019725412E-7</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -3113,13 +3113,13 @@
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B69" s="2">
         <v>1.8431983348741521E-7</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -3127,13 +3127,13 @@
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B70" s="2">
         <v>0.01</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -3141,13 +3141,13 @@
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B71" s="2">
         <v>1.4778797459801761E-7</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -3155,13 +3155,13 @@
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B72" s="2">
         <v>0.01</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -3169,13 +3169,13 @@
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B73" s="2">
         <v>1.7767767732570659E-7</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -3183,13 +3183,13 @@
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B74" s="2">
         <v>0.01</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -3197,13 +3197,13 @@
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B75" s="2">
         <v>1.4114581843630891E-7</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -3211,13 +3211,13 @@
     </row>
     <row r="76" spans="1:6" ht="15" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B76" s="2">
         <v>0.01</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -3225,13 +3225,13 @@
     </row>
     <row r="77" spans="1:6" ht="15" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B77" s="2">
         <v>1.7103552116399789E-7</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -3239,13 +3239,13 @@
     </row>
     <row r="78" spans="1:6" ht="15" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B78" s="2">
         <v>0.01</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -3253,13 +3253,13 @@
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B79" s="2">
         <v>1.6273282596186211E-7</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -3267,13 +3267,13 @@
     </row>
     <row r="80" spans="1:6" ht="15" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B80" s="2">
         <v>0.01</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -3281,13 +3281,13 @@
     </row>
     <row r="81" spans="1:6" ht="15" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B81" s="2">
         <v>2.042463019725412E-7</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -3295,13 +3295,13 @@
     </row>
     <row r="82" spans="1:6" ht="15" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B82" s="2">
         <v>0.01</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -3309,13 +3309,13 @@
     </row>
     <row r="83" spans="1:6" ht="15" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B83" s="2">
         <v>1.5443013075972631E-7</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -3323,13 +3323,13 @@
     </row>
     <row r="84" spans="1:6" ht="15" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B84" s="2">
         <v>0.01</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -3337,13 +3337,13 @@
     </row>
     <row r="85" spans="1:6" ht="15" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B85" s="2">
         <v>1.2454042803203729E-7</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -3351,13 +3351,13 @@
     </row>
     <row r="86" spans="1:6" ht="15" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B86" s="2">
         <v>0.01</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -3365,13 +3365,13 @@
     </row>
     <row r="87" spans="1:6" ht="15" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B87" s="2">
         <v>1.9262252868955099E-7</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -3379,13 +3379,13 @@
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B88" s="2">
         <v>0.01</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -3393,13 +3393,13 @@
     </row>
     <row r="89" spans="1:6" ht="15" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B89" s="2">
         <v>1.428063574767361E-7</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -3407,13 +3407,13 @@
     </row>
     <row r="90" spans="1:6" ht="15" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B90" s="2">
         <v>0.01</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -3421,13 +3421,13 @@
     </row>
     <row r="91" spans="1:6" ht="15" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B91" s="2">
         <v>1.3450366227460029E-7</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -3435,13 +3435,13 @@
     </row>
     <row r="92" spans="1:6" ht="15" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B92" s="2">
         <v>0.01</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -3449,13 +3449,13 @@
     </row>
     <row r="93" spans="1:6" ht="15" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B93" s="2">
         <v>6.7999999999999999E-5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -3463,13 +3463,13 @@
     </row>
     <row r="94" spans="1:6" ht="15" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B94" s="2">
         <v>6.7999999999999999E-5</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -3477,13 +3477,13 @@
     </row>
     <row r="95" spans="1:6" ht="15" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B95" s="2">
         <v>1.8000000000000001E-4</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -3491,13 +3491,13 @@
     </row>
     <row r="96" spans="1:6" ht="15" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B96" s="2">
         <v>1.8000000000000001E-4</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -3505,13 +3505,13 @@
     </row>
     <row r="97" spans="1:6" ht="15" customHeight="1">
       <c r="A97" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B97" s="2">
         <v>1.2E-5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -3519,13 +3519,13 @@
     </row>
     <row r="98" spans="1:6" ht="15" customHeight="1">
       <c r="A98" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B98" s="2">
         <v>1.2E-5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -3533,13 +3533,13 @@
     </row>
     <row r="99" spans="1:6" ht="15" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B99" s="2">
         <v>2.9E-5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -3547,13 +3547,13 @@
     </row>
     <row r="100" spans="1:6" ht="15" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B100" s="2">
         <v>2.9E-5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -3561,13 +3561,13 @@
     </row>
     <row r="101" spans="1:6" ht="15" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B101" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -3575,13 +3575,13 @@
     </row>
     <row r="102" spans="1:6" ht="15" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B102" s="2">
         <v>2E-3</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -3589,13 +3589,13 @@
     </row>
     <row r="103" spans="1:6" ht="15" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B103" s="2">
         <v>8.3329999999999997E-6</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -3603,13 +3603,13 @@
     </row>
     <row r="104" spans="1:6" ht="15" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B104" s="2">
         <v>2E-3</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -3617,13 +3617,13 @@
     </row>
     <row r="105" spans="1:6" ht="15" customHeight="1">
       <c r="A105" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B105" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -3631,13 +3631,13 @@
     </row>
     <row r="106" spans="1:6" ht="15" customHeight="1">
       <c r="A106" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B106" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -3660,7 +3660,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -3670,13 +3670,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -3705,23 +3705,23 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -3747,7 +3747,7 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -3757,13 +3757,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>11</v>
@@ -3772,7 +3772,7 @@
         <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -3791,7 +3791,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -3801,10 +3801,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>11</v>
@@ -3818,14 +3818,14 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
         <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3833,14 +3833,14 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
         <v>1000000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -3848,14 +3848,14 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
         <v>0.3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -3863,14 +3863,14 @@
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
         <v>1.0000000000000001E-15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3893,7 +3893,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -3903,13 +3903,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>370</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -3923,16 +3923,16 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>372</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3941,16 +3941,16 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -3959,16 +3959,16 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -3977,16 +3977,16 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3995,16 +3995,16 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -4013,16 +4013,16 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -4031,16 +4031,16 @@
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -4049,16 +4049,16 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -4067,16 +4067,16 @@
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -4085,16 +4085,16 @@
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4103,16 +4103,16 @@
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -4136,14 +4136,14 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -4163,7 +4163,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4208,7 +4208,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4271,7 +4271,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4820,10 +4820,10 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4833,16 +4833,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>22</v>
@@ -4859,10 +4859,10 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="b">
@@ -4896,32 +4896,32 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -4950,32 +4950,32 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -4989,16 +4989,16 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2">
@@ -5008,7 +5008,7 @@
         <v>137</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -5016,16 +5016,16 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
@@ -5035,7 +5035,7 @@
         <v>335</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -5043,16 +5043,16 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2">
@@ -5062,7 +5062,7 @@
         <v>497</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -5070,16 +5070,16 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2">
@@ -5089,7 +5089,7 @@
         <v>856</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -5097,16 +5097,16 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2">
@@ -5116,7 +5116,7 @@
         <v>1046</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -5124,16 +5124,16 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2">
@@ -5143,7 +5143,7 @@
         <v>1260</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -5151,16 +5151,16 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2">
@@ -5170,7 +5170,7 @@
         <v>1412</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -5178,16 +5178,16 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2">
@@ -5197,7 +5197,7 @@
         <v>1570</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -5205,16 +5205,16 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2">
@@ -5224,7 +5224,7 @@
         <v>1730</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -5232,16 +5232,16 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2">
@@ -5251,7 +5251,7 @@
         <v>1884</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -5259,16 +5259,16 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
@@ -5278,7 +5278,7 @@
         <v>2547</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -5286,16 +5286,16 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
@@ -5305,7 +5305,7 @@
         <v>2753</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -5328,7 +5328,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -5338,16 +5338,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>22</v>
@@ -5364,16 +5364,16 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>0</v>
@@ -5390,16 +5390,16 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>0</v>
@@ -5416,16 +5416,16 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" s="2" t="b">
         <v>0</v>
@@ -5442,16 +5442,16 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E5" s="2" t="b">
         <v>0</v>
@@ -5468,16 +5468,16 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" s="2" t="b">
         <v>0</v>
@@ -5494,16 +5494,16 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>0</v>
@@ -5520,16 +5520,16 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>0</v>
@@ -5546,16 +5546,16 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
@@ -5572,16 +5572,16 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>0</v>
@@ -5598,16 +5598,16 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
@@ -5624,16 +5624,16 @@
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
@@ -5650,16 +5650,16 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
@@ -5691,32 +5691,32 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -5730,20 +5730,20 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G2" s="2">
         <v>9</v>
@@ -5757,20 +5757,20 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G3" s="2">
         <v>159</v>
@@ -5784,20 +5784,20 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G4" s="2">
         <v>354</v>
@@ -5811,20 +5811,20 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G5" s="2">
         <v>522</v>
@@ -5838,20 +5838,20 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" s="2">
         <v>687</v>
@@ -5865,20 +5865,20 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" s="2">
         <v>870</v>
@@ -5892,20 +5892,20 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G8" s="2">
         <v>1074</v>
@@ -5919,20 +5919,20 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G9" s="2">
         <v>1281</v>
@@ -5946,20 +5946,20 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G10" s="2">
         <v>1419</v>
@@ -5973,20 +5973,20 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G11" s="2">
         <v>1593</v>
@@ -6000,20 +6000,20 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G12" s="2">
         <v>1752</v>
@@ -6027,20 +6027,20 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G13" s="2">
         <v>1911</v>
@@ -6054,20 +6054,20 @@
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
       <c r="A14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G14" s="2">
         <v>2061</v>
@@ -6081,20 +6081,20 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G15" s="2">
         <v>2235</v>
@@ -6108,20 +6108,20 @@
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G16" s="2">
         <v>2415</v>
@@ -6135,20 +6135,20 @@
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G17" s="2">
         <v>2577</v>

</xml_diff>

<commit_message>
debugging; fixing transcription reaction stochiometries; updating for removal of specific parameters in wc-sim/models
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -1147,7 +1147,7 @@
     <t>Database References</t>
   </si>
   <si>
-    <t>cell_cycle_len</t>
+    <t>mean_doubling_time</t>
   </si>
   <si>
     <t>s</t>
@@ -1165,7 +1165,7 @@
     <t>dimensionless</t>
   </si>
   <si>
-    <t>initial_volume</t>
+    <t>mean_volume</t>
   </si>
   <si>
     <t>L</t>
@@ -1248,12 +1248,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1275,14 +1275,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1291,9 +1283,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1307,11 +1298,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1323,7 +1344,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1337,30 +1404,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1368,59 +1414,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1453,7 +1446,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1465,7 +1500,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1478,162 +1627,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1656,6 +1649,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1671,35 +1688,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1730,165 +1729,159 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4454,7 +4447,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
Modify rate law representation due to changes in RateLawExpression in wc_kb
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19800" windowHeight="6840" tabRatio="865" firstSheet="8" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19800" windowHeight="6840" tabRatio="865" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="400">
   <si>
     <t>Id</t>
   </si>
@@ -1132,15 +1132,6 @@
     <t>Direction</t>
   </si>
   <si>
-    <t>Equation</t>
-  </si>
-  <si>
-    <t>K cat</t>
-  </si>
-  <si>
-    <t>K m</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -1256,6 +1247,9 @@
   </si>
   <si>
     <t>Expression</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -3714,30 +3708,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>360</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>361</v>
+        <v>398</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>362</v>
+        <v>248</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -3776,7 +3770,7 @@
         <v>247</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>248</v>
@@ -3788,7 +3782,7 @@
         <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3834,14 +3828,14 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
         <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3849,14 +3843,14 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
         <v>1000000</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -3864,14 +3858,14 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
         <v>0.3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -3879,14 +3873,14 @@
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
         <v>1.0000000000000001E-15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3902,7 +3896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -3919,7 +3913,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>248</v>
@@ -3936,10 +3930,10 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>311</v>
@@ -3953,10 +3947,10 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>309</v>
@@ -3970,7 +3964,7 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>244</v>
@@ -3987,10 +3981,10 @@
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>312</v>
@@ -4004,10 +3998,10 @@
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>314</v>
@@ -4021,10 +4015,10 @@
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>306</v>
@@ -4038,10 +4032,10 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>305</v>
@@ -4055,10 +4049,10 @@
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>325</v>
@@ -4072,10 +4066,10 @@
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>321</v>
@@ -4089,10 +4083,10 @@
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>317</v>
@@ -4106,10 +4100,10 @@
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>339</v>
@@ -4145,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -4815,24 +4809,24 @@
     </row>
     <row r="36" spans="1:7" ht="60">
       <c r="A36" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30">
       <c r="A37" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C37" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert changing structure property type in fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -2437,7 +2437,7 @@
     <t>!Year</t>
   </si>
   <si>
-    <t>inchi_structure</t>
+    <t>structure</t>
   </si>
 </sst>
 </file>
@@ -4340,10 +4340,10 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E106" sqref="E106"/>
+      <selection pane="bottomRight" activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updating fixture for changes to obj_tables and wc_kb
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_model_kb.xlsx
+++ b/tests/fixtures/min_model_kb.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="11" autoFilterDateGrouping="1" firstSheet="5" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="886" visibility="visible" windowHeight="13965" windowWidth="28695" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13965" tabRatio="886" firstSheet="5" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!KB" sheetId="1" state="visible" r:id="rId1"/>
@@ -28,22 +28,22 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!References" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'!!KB'!$A$1:$B$9</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'!!Cell'!$A$1:$B$4</definedName>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'!!Compartments'!$A$1:$E$3</definedName>
-    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">'!!Chromosomes'!$A$1:$I$2</definedName>
-    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'!!Transcription units'!$A$1:$L$28</definedName>
-    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'!!Genes'!$A$1:$I$37</definedName>
-    <definedName hidden="1" localSheetId="7" name="_xlnm._FilterDatabase">'!!RNAs'!$A$1:$J$28</definedName>
-    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'!!Proteins'!$A$1:$G$37</definedName>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">'!!Complexes'!$A$1:$F$2</definedName>
-    <definedName hidden="1" localSheetId="10" name="_xlnm._FilterDatabase">'!!Metabolites'!$A$1:$G$37</definedName>
-    <definedName hidden="1" localSheetId="11" name="_xlnm._FilterDatabase">'!!Species type properties'!$A$1:$J$100</definedName>
-    <definedName hidden="1" localSheetId="12" name="_xlnm._FilterDatabase">'!!Concentrations'!$B$1:$F$101</definedName>
-    <definedName hidden="1" localSheetId="13" name="_xlnm._FilterDatabase">'!!Observables'!$A$1:$F$13</definedName>
-    <definedName hidden="1" localSheetId="14" name="_xlnm._FilterDatabase">'!!Reactions'!$A$1:$J$3</definedName>
-    <definedName hidden="1" localSheetId="15" name="_xlnm._FilterDatabase">'!!Rate laws'!$A$1:$G$3</definedName>
-    <definedName hidden="1" localSheetId="19" name="_xlnm._FilterDatabase">'!!References'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!KB'!$A$1:$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!!Cell'!$A$1:$B$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!!Compartments'!$A$1:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'!!Chromosomes'!$A$1:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'!!Transcription units'!$A$1:$L$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!!Genes'!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'!!RNAs'!$A$1:$J$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'!!Proteins'!$A$1:$G$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'!!Complexes'!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'!!Metabolites'!$A$1:$G$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'!!Species type properties'!$A$1:$J$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'!!Concentrations'!$B$1:$F$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'!!Observables'!$A$1:$F$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'!!Reactions'!$A$1:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'!!Rate laws'!$A$1:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'!!References'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -277,338 +277,338 @@
     </border>
   </borders>
   <cellStyleXfs count="78">
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="89">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="11" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="2" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="8" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="35">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="35">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="35">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="35">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="35">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="35">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="35">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="35">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="31"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="28">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="28">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="28">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="28">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="10" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="31">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31"/>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="31"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="31">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="31">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="31">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="31">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="31">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="78">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 9 4" xfId="1"/>
     <cellStyle name="Normal 9 3" xfId="2"/>
     <cellStyle name="Normal 9 2 2" xfId="3"/>
@@ -687,7 +687,7 @@
     <cellStyle name="Normal 6 5 3" xfId="76"/>
     <cellStyle name="Normal 6 3 4" xfId="77"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -983,35 +983,35 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="D14" pane="bottomRight" sqref="D14"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="22"/>
-    <col customWidth="1" max="2" min="2" style="15" width="16.28515625"/>
-    <col customWidth="1" max="3" min="3" style="15" width="9"/>
-    <col customWidth="1" max="16384" min="4" style="15" width="9"/>
+    <col width="22" customWidth="1" style="15" min="1" max="1"/>
+    <col width="16.28515625" customWidth="1" style="15" min="2" max="2"/>
+    <col width="9" customWidth="1" style="15" min="3" max="3"/>
+    <col width="9" customWidth="1" style="15" min="4" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!!ObjTables objTablesVersion='0.0.8'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='KnowledgeBase' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="3">
+          <t>!!ObjTables type='Data' id='KnowledgeBase' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="column"</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="30" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -1023,7 +1023,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="83" t="inlineStr">
         <is>
           <t>!Name</t>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B4" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="83" t="inlineStr">
         <is>
           <t>!Translation table</t>
@@ -1041,7 +1041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="84" t="inlineStr">
         <is>
           <t>!Version</t>
@@ -1096,7 +1096,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B9"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1109,25 +1109,25 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="N20" pane="bottomRight" sqref="N20"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="9" min="1" style="15" width="15.7109375"/>
+    <col width="15.7109375" customWidth="1" style="15" min="1" max="9"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='ComplexSpeciesType' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='ComplexSpeciesType' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="31" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -1178,7 +1178,7 @@
       <c r="L2" s="29" t="n"/>
       <c r="M2" s="29" t="n"/>
     </row>
-    <row customHeight="1" ht="25.5" r="3">
+    <row r="3" ht="25.5" customHeight="1">
       <c r="A3" s="43" t="inlineStr">
         <is>
           <t>ribosome</t>
@@ -1473,7 +1473,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F2"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1486,29 +1486,29 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B17" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="J68" pane="bottomRight" sqref="J68:J70"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="J68" sqref="J68:J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="45" width="15.7109375"/>
-    <col customWidth="1" max="2" min="2" style="45" width="25.7109375"/>
-    <col customWidth="1" max="7" min="3" style="45" width="15.7109375"/>
-    <col customWidth="1" max="8" min="8" style="45" width="9"/>
-    <col customWidth="1" max="16384" min="9" style="45" width="9"/>
+    <col width="15.7109375" customWidth="1" style="45" min="1" max="1"/>
+    <col width="25.7109375" customWidth="1" style="45" min="2" max="2"/>
+    <col width="15.7109375" customWidth="1" style="45" min="3" max="7"/>
+    <col width="9" customWidth="1" style="45" min="8" max="8"/>
+    <col width="9" customWidth="1" style="45" min="9" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="8">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='MetaboliteSpeciesType' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='MetaboliteSpeciesType' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -1545,7 +1545,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="46" t="inlineStr">
         <is>
           <t>adp</t>
@@ -1562,7 +1562,7 @@
       <c r="F3" s="47" t="n"/>
       <c r="G3" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="46" t="inlineStr">
         <is>
           <t>ala</t>
@@ -1579,7 +1579,7 @@
       <c r="F4" s="47" t="n"/>
       <c r="G4" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="46" t="inlineStr">
         <is>
           <t>amp</t>
@@ -1596,7 +1596,7 @@
       <c r="F5" s="47" t="n"/>
       <c r="G5" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="46" t="inlineStr">
         <is>
           <t>arg</t>
@@ -1613,7 +1613,7 @@
       <c r="F6" s="47" t="n"/>
       <c r="G6" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="7">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="46" t="inlineStr">
         <is>
           <t>asn</t>
@@ -1630,7 +1630,7 @@
       <c r="F7" s="47" t="n"/>
       <c r="G7" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="8">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="46" t="inlineStr">
         <is>
           <t>asp</t>
@@ -1647,7 +1647,7 @@
       <c r="F8" s="47" t="n"/>
       <c r="G8" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="9">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="46" t="inlineStr">
         <is>
           <t>atp</t>
@@ -1664,7 +1664,7 @@
       <c r="F9" s="47" t="n"/>
       <c r="G9" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="10">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="46" t="inlineStr">
         <is>
           <t>cmp</t>
@@ -1681,7 +1681,7 @@
       <c r="F10" s="47" t="n"/>
       <c r="G10" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="11">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="46" t="inlineStr">
         <is>
           <t>cdp</t>
@@ -1698,7 +1698,7 @@
       <c r="F11" s="47" t="n"/>
       <c r="G11" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="12">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="46" t="inlineStr">
         <is>
           <t>ctp</t>
@@ -1715,7 +1715,7 @@
       <c r="F12" s="47" t="n"/>
       <c r="G12" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="13">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="46" t="inlineStr">
         <is>
           <t>cys</t>
@@ -1732,7 +1732,7 @@
       <c r="F13" s="47" t="n"/>
       <c r="G13" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="14">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="46" t="inlineStr">
         <is>
           <t>gdp</t>
@@ -1749,7 +1749,7 @@
       <c r="F14" s="47" t="n"/>
       <c r="G14" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="15">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="46" t="inlineStr">
         <is>
           <t>gln</t>
@@ -1766,7 +1766,7 @@
       <c r="F15" s="47" t="n"/>
       <c r="G15" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="16">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="46" t="inlineStr">
         <is>
           <t>glu</t>
@@ -1783,7 +1783,7 @@
       <c r="F16" s="47" t="n"/>
       <c r="G16" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="17">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="46" t="inlineStr">
         <is>
           <t>gly</t>
@@ -1800,7 +1800,7 @@
       <c r="F17" s="47" t="n"/>
       <c r="G17" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="18">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="46" t="inlineStr">
         <is>
           <t>gmp</t>
@@ -1817,7 +1817,7 @@
       <c r="F18" s="47" t="n"/>
       <c r="G18" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="19">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="46" t="inlineStr">
         <is>
           <t>gtp</t>
@@ -1834,7 +1834,7 @@
       <c r="F19" s="47" t="n"/>
       <c r="G19" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="20">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="46" t="inlineStr">
         <is>
           <t>h</t>
@@ -1851,7 +1851,7 @@
       <c r="F20" s="47" t="n"/>
       <c r="G20" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="21">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="46" t="inlineStr">
         <is>
           <t>h2o</t>
@@ -1868,7 +1868,7 @@
       <c r="F21" s="47" t="n"/>
       <c r="G21" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="22">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="46" t="inlineStr">
         <is>
           <t>his</t>
@@ -1885,7 +1885,7 @@
       <c r="F22" s="47" t="n"/>
       <c r="G22" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="23">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="46" t="inlineStr">
         <is>
           <t>ile</t>
@@ -1902,7 +1902,7 @@
       <c r="F23" s="47" t="n"/>
       <c r="G23" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="24">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="46" t="inlineStr">
         <is>
           <t>leu</t>
@@ -1919,7 +1919,7 @@
       <c r="F24" s="47" t="n"/>
       <c r="G24" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="25">
+    <row r="25" ht="15" customHeight="1">
       <c r="A25" s="46" t="inlineStr">
         <is>
           <t>lys</t>
@@ -1936,7 +1936,7 @@
       <c r="F25" s="47" t="n"/>
       <c r="G25" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="26">
+    <row r="26" ht="15" customHeight="1">
       <c r="A26" s="46" t="inlineStr">
         <is>
           <t>met</t>
@@ -1953,7 +1953,7 @@
       <c r="F26" s="47" t="n"/>
       <c r="G26" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="27">
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" s="46" t="inlineStr">
         <is>
           <t>phe</t>
@@ -1970,7 +1970,7 @@
       <c r="F27" s="47" t="n"/>
       <c r="G27" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="28">
+    <row r="28" ht="15" customHeight="1">
       <c r="A28" s="46" t="inlineStr">
         <is>
           <t>pi</t>
@@ -1987,7 +1987,7 @@
       <c r="F28" s="47" t="n"/>
       <c r="G28" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="29">
+    <row r="29" ht="15" customHeight="1">
       <c r="A29" s="46" t="inlineStr">
         <is>
           <t>ppi</t>
@@ -2004,7 +2004,7 @@
       <c r="F29" s="47" t="n"/>
       <c r="G29" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="30">
+    <row r="30" ht="15" customHeight="1">
       <c r="A30" s="46" t="inlineStr">
         <is>
           <t>pro</t>
@@ -2021,7 +2021,7 @@
       <c r="F30" s="47" t="n"/>
       <c r="G30" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="31">
+    <row r="31" ht="15" customHeight="1">
       <c r="A31" s="46" t="inlineStr">
         <is>
           <t>ser</t>
@@ -2038,7 +2038,7 @@
       <c r="F31" s="47" t="n"/>
       <c r="G31" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="32">
+    <row r="32" ht="15" customHeight="1">
       <c r="A32" s="46" t="inlineStr">
         <is>
           <t>thr</t>
@@ -2055,7 +2055,7 @@
       <c r="F32" s="47" t="n"/>
       <c r="G32" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="33">
+    <row r="33" ht="15" customHeight="1">
       <c r="A33" s="46" t="inlineStr">
         <is>
           <t>trp</t>
@@ -2072,7 +2072,7 @@
       <c r="F33" s="47" t="n"/>
       <c r="G33" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="34">
+    <row r="34" ht="15" customHeight="1">
       <c r="A34" s="46" t="inlineStr">
         <is>
           <t>tyr</t>
@@ -2089,7 +2089,7 @@
       <c r="F34" s="47" t="n"/>
       <c r="G34" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="35">
+    <row r="35" ht="15" customHeight="1">
       <c r="A35" s="46" t="inlineStr">
         <is>
           <t>ump</t>
@@ -2106,7 +2106,7 @@
       <c r="F35" s="47" t="n"/>
       <c r="G35" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="36">
+    <row r="36" ht="15" customHeight="1">
       <c r="A36" s="46" t="inlineStr">
         <is>
           <t>udp</t>
@@ -2123,7 +2123,7 @@
       <c r="F36" s="47" t="n"/>
       <c r="G36" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="37">
+    <row r="37" ht="15" customHeight="1">
       <c r="A37" s="46" t="inlineStr">
         <is>
           <t>utp</t>
@@ -2159,7 +2159,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G37"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2172,23 +2172,23 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B53" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="H74" pane="bottomRight" sqref="H74"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="30.7109375"/>
-    <col customWidth="1" max="2" min="2" style="38" width="15.7109375"/>
-    <col customWidth="1" max="11" min="3" style="9" width="15.7109375"/>
+    <col width="30.7109375" customWidth="1" style="11" min="1" max="1"/>
+    <col width="15.7109375" customWidth="1" style="38" min="2" max="2"/>
+    <col width="15.7109375" customWidth="1" style="9" min="3" max="11"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="37">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="37">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='SpeciesTypeProperty' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='SpeciesTypeProperty' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
         </is>
       </c>
     </row>
@@ -5285,7 +5285,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J100"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -5298,30 +5298,30 @@
   <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="C59" xSplit="2" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="F46" pane="bottomRight" sqref="F46"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="37.42578125"/>
-    <col customWidth="1" max="2" min="2" style="15" width="20.7109375"/>
-    <col customWidth="1" max="4" min="3" style="24" width="15.7109375"/>
-    <col customWidth="1" max="8" min="5" style="15" width="15.7109375"/>
-    <col customWidth="1" max="9" min="9" style="15" width="9"/>
-    <col customWidth="1" max="16384" min="10" style="15" width="9"/>
+    <col width="37.42578125" customWidth="1" style="15" min="1" max="1"/>
+    <col width="20.7109375" customWidth="1" style="15" min="2" max="2"/>
+    <col width="15.7109375" customWidth="1" style="24" min="3" max="4"/>
+    <col width="15.7109375" customWidth="1" style="15" min="5" max="8"/>
+    <col width="9" customWidth="1" style="15" min="9" max="9"/>
+    <col width="9" customWidth="1" style="15" min="10" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="34">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="34">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Concentration' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='Concentration' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
           <t>!ID</t>
@@ -5363,7 +5363,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>CONC(adp[c])</t>
@@ -5385,7 +5385,7 @@
       <c r="E3" s="14" t="n"/>
       <c r="F3" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>CONC(ala[c])</t>
@@ -5407,7 +5407,7 @@
       <c r="E4" s="14" t="n"/>
       <c r="F4" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>CONC(amp[c])</t>
@@ -5429,7 +5429,7 @@
       <c r="E5" s="14" t="n"/>
       <c r="F5" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="15" t="inlineStr">
         <is>
           <t>CONC(arg[c])</t>
@@ -5451,7 +5451,7 @@
       <c r="E6" s="14" t="n"/>
       <c r="F6" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="7">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="15" t="inlineStr">
         <is>
           <t>CONC(asn[c])</t>
@@ -5473,7 +5473,7 @@
       <c r="E7" s="14" t="n"/>
       <c r="F7" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="8">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>CONC(asp[c])</t>
@@ -5495,7 +5495,7 @@
       <c r="E8" s="14" t="n"/>
       <c r="F8" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="9">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="15" t="inlineStr">
         <is>
           <t>CONC(atp[c])</t>
@@ -5517,7 +5517,7 @@
       <c r="E9" s="14" t="n"/>
       <c r="F9" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="10">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="15" t="inlineStr">
         <is>
           <t>CONC(cmp[c])</t>
@@ -5539,7 +5539,7 @@
       <c r="E10" s="14" t="n"/>
       <c r="F10" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="11">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="15" t="inlineStr">
         <is>
           <t>CONC(cdp[c])</t>
@@ -5561,7 +5561,7 @@
       <c r="E11" s="14" t="n"/>
       <c r="F11" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="12">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="15" t="inlineStr">
         <is>
           <t>CONC(ctp[c])</t>
@@ -5583,7 +5583,7 @@
       <c r="E12" s="14" t="n"/>
       <c r="F12" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="13">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="15" t="inlineStr">
         <is>
           <t>CONC(cys[c])</t>
@@ -5605,7 +5605,7 @@
       <c r="E13" s="14" t="n"/>
       <c r="F13" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="14">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="15" t="inlineStr">
         <is>
           <t>CONC(gdp[c])</t>
@@ -5627,7 +5627,7 @@
       <c r="E14" s="14" t="n"/>
       <c r="F14" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="15">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="15" t="inlineStr">
         <is>
           <t>CONC(gln[c])</t>
@@ -5649,7 +5649,7 @@
       <c r="E15" s="14" t="n"/>
       <c r="F15" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="16">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="15" t="inlineStr">
         <is>
           <t>CONC(glu[c])</t>
@@ -5671,7 +5671,7 @@
       <c r="E16" s="14" t="n"/>
       <c r="F16" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="17">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="15" t="inlineStr">
         <is>
           <t>CONC(gly[c])</t>
@@ -5693,7 +5693,7 @@
       <c r="E17" s="14" t="n"/>
       <c r="F17" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="18">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="15" t="inlineStr">
         <is>
           <t>CONC(gmp[c])</t>
@@ -5715,7 +5715,7 @@
       <c r="E18" s="14" t="n"/>
       <c r="F18" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="19">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="15" t="inlineStr">
         <is>
           <t>CONC(gtp[c])</t>
@@ -5737,7 +5737,7 @@
       <c r="E19" s="14" t="n"/>
       <c r="F19" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="20">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="15" t="inlineStr">
         <is>
           <t>CONC(h2o[c])</t>
@@ -5759,7 +5759,7 @@
       <c r="E20" s="14" t="n"/>
       <c r="F20" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="21">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="15" t="inlineStr">
         <is>
           <t>CONC(h[c])</t>
@@ -5781,7 +5781,7 @@
       <c r="E21" s="14" t="n"/>
       <c r="F21" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="22">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="15" t="inlineStr">
         <is>
           <t>CONC(his[c])</t>
@@ -5803,7 +5803,7 @@
       <c r="E22" s="14" t="n"/>
       <c r="F22" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="23">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="15" t="inlineStr">
         <is>
           <t>CONC(ile[c])</t>
@@ -5825,7 +5825,7 @@
       <c r="E23" s="14" t="n"/>
       <c r="F23" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="24">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="15" t="inlineStr">
         <is>
           <t>CONC(leu[c])</t>
@@ -5847,7 +5847,7 @@
       <c r="E24" s="14" t="n"/>
       <c r="F24" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="25">
+    <row r="25" ht="15" customHeight="1">
       <c r="A25" s="15" t="inlineStr">
         <is>
           <t>CONC(lys[c])</t>
@@ -5869,7 +5869,7 @@
       <c r="E25" s="14" t="n"/>
       <c r="F25" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="26">
+    <row r="26" ht="15" customHeight="1">
       <c r="A26" s="15" t="inlineStr">
         <is>
           <t>CONC(met[c])</t>
@@ -5891,7 +5891,7 @@
       <c r="E26" s="14" t="n"/>
       <c r="F26" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="27">
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" s="15" t="inlineStr">
         <is>
           <t>CONC(phe[c])</t>
@@ -5913,7 +5913,7 @@
       <c r="E27" s="14" t="n"/>
       <c r="F27" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="28">
+    <row r="28" ht="15" customHeight="1">
       <c r="A28" s="15" t="inlineStr">
         <is>
           <t>CONC(pi[c])</t>
@@ -5935,7 +5935,7 @@
       <c r="E28" s="14" t="n"/>
       <c r="F28" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="29">
+    <row r="29" ht="15" customHeight="1">
       <c r="A29" s="15" t="inlineStr">
         <is>
           <t>CONC(ppi[c])</t>
@@ -5957,7 +5957,7 @@
       <c r="E29" s="14" t="n"/>
       <c r="F29" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="30">
+    <row r="30" ht="15" customHeight="1">
       <c r="A30" s="15" t="inlineStr">
         <is>
           <t>CONC(pro[c])</t>
@@ -5979,7 +5979,7 @@
       <c r="E30" s="14" t="n"/>
       <c r="F30" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="31">
+    <row r="31" ht="15" customHeight="1">
       <c r="A31" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_1[c])</t>
@@ -6001,7 +6001,7 @@
       <c r="E31" s="14" t="n"/>
       <c r="F31" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="32">
+    <row r="32" ht="15" customHeight="1">
       <c r="A32" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_2[c])</t>
@@ -6023,7 +6023,7 @@
       <c r="E32" s="14" t="n"/>
       <c r="F32" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="33">
+    <row r="33" ht="15" customHeight="1">
       <c r="A33" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_3[c])</t>
@@ -6045,7 +6045,7 @@
       <c r="E33" s="14" t="n"/>
       <c r="F33" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="34">
+    <row r="34" ht="15" customHeight="1">
       <c r="A34" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_4[c])</t>
@@ -6067,7 +6067,7 @@
       <c r="E34" s="14" t="n"/>
       <c r="F34" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="35">
+    <row r="35" ht="15" customHeight="1">
       <c r="A35" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_5[c])</t>
@@ -6089,7 +6089,7 @@
       <c r="E35" s="14" t="n"/>
       <c r="F35" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="36">
+    <row r="36" ht="15" customHeight="1">
       <c r="A36" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_6[c])</t>
@@ -6111,7 +6111,7 @@
       <c r="E36" s="14" t="n"/>
       <c r="F36" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="37">
+    <row r="37" ht="15" customHeight="1">
       <c r="A37" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_7[c])</t>
@@ -6133,7 +6133,7 @@
       <c r="E37" s="14" t="n"/>
       <c r="F37" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="38">
+    <row r="38" ht="15" customHeight="1">
       <c r="A38" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_8[c])</t>
@@ -6155,7 +6155,7 @@
       <c r="E38" s="14" t="n"/>
       <c r="F38" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="39">
+    <row r="39" ht="15" customHeight="1">
       <c r="A39" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_9[c])</t>
@@ -6177,7 +6177,7 @@
       <c r="E39" s="14" t="n"/>
       <c r="F39" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="40">
+    <row r="40" ht="15" customHeight="1">
       <c r="A40" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_10[c])</t>
@@ -6199,7 +6199,7 @@
       <c r="E40" s="14" t="n"/>
       <c r="F40" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="41">
+    <row r="41" ht="15" customHeight="1">
       <c r="A41" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_11[c])</t>
@@ -6221,7 +6221,7 @@
       <c r="E41" s="14" t="n"/>
       <c r="F41" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="42">
+    <row r="42" ht="15" customHeight="1">
       <c r="A42" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_12[c])</t>
@@ -6243,7 +6243,7 @@
       <c r="E42" s="14" t="n"/>
       <c r="F42" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="43">
+    <row r="43" ht="15" customHeight="1">
       <c r="A43" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_13[c])</t>
@@ -6265,7 +6265,7 @@
       <c r="E43" s="14" t="n"/>
       <c r="F43" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="44">
+    <row r="44" ht="15" customHeight="1">
       <c r="A44" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_14[c])</t>
@@ -6287,7 +6287,7 @@
       <c r="E44" s="14" t="n"/>
       <c r="F44" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="45">
+    <row r="45" ht="15" customHeight="1">
       <c r="A45" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_15[c])</t>
@@ -6309,7 +6309,7 @@
       <c r="E45" s="14" t="n"/>
       <c r="F45" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="46">
+    <row r="46" ht="15" customHeight="1">
       <c r="A46" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_16[c])</t>
@@ -6331,7 +6331,7 @@
       <c r="E46" s="14" t="n"/>
       <c r="F46" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="47">
+    <row r="47" ht="15" customHeight="1">
       <c r="A47" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_17[c])</t>
@@ -6353,7 +6353,7 @@
       <c r="E47" s="14" t="n"/>
       <c r="F47" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="48">
+    <row r="48" ht="15" customHeight="1">
       <c r="A48" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_18[c])</t>
@@ -6375,7 +6375,7 @@
       <c r="E48" s="14" t="n"/>
       <c r="F48" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="49">
+    <row r="49" ht="15" customHeight="1">
       <c r="A49" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_19[c])</t>
@@ -6397,7 +6397,7 @@
       <c r="E49" s="14" t="n"/>
       <c r="F49" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="50">
+    <row r="50" ht="15" customHeight="1">
       <c r="A50" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_20[c])</t>
@@ -6419,7 +6419,7 @@
       <c r="E50" s="14" t="n"/>
       <c r="F50" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="51">
+    <row r="51" ht="15" customHeight="1">
       <c r="A51" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_21[c])</t>
@@ -6441,7 +6441,7 @@
       <c r="E51" s="14" t="n"/>
       <c r="F51" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="52">
+    <row r="52" ht="15" customHeight="1">
       <c r="A52" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_22[c])</t>
@@ -6463,7 +6463,7 @@
       <c r="E52" s="14" t="n"/>
       <c r="F52" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="53">
+    <row r="53" ht="15" customHeight="1">
       <c r="A53" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_23[c])</t>
@@ -6485,7 +6485,7 @@
       <c r="E53" s="14" t="n"/>
       <c r="F53" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="54">
+    <row r="54" ht="15" customHeight="1">
       <c r="A54" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_24[c])</t>
@@ -6507,7 +6507,7 @@
       <c r="E54" s="14" t="n"/>
       <c r="F54" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="55">
+    <row r="55" ht="15" customHeight="1">
       <c r="A55" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_25[c])</t>
@@ -6529,7 +6529,7 @@
       <c r="E55" s="14" t="n"/>
       <c r="F55" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="56">
+    <row r="56" ht="15" customHeight="1">
       <c r="A56" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_26[c])</t>
@@ -6551,7 +6551,7 @@
       <c r="E56" s="14" t="n"/>
       <c r="F56" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="57">
+    <row r="57" ht="15" customHeight="1">
       <c r="A57" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_27[c])</t>
@@ -6573,7 +6573,7 @@
       <c r="E57" s="14" t="n"/>
       <c r="F57" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="58">
+    <row r="58" ht="15" customHeight="1">
       <c r="A58" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_28[c])</t>
@@ -6595,7 +6595,7 @@
       <c r="E58" s="14" t="n"/>
       <c r="F58" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="59">
+    <row r="59" ht="15" customHeight="1">
       <c r="A59" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_29[c])</t>
@@ -6617,7 +6617,7 @@
       <c r="E59" s="14" t="n"/>
       <c r="F59" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="60">
+    <row r="60" ht="15" customHeight="1">
       <c r="A60" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_30[c])</t>
@@ -6639,7 +6639,7 @@
       <c r="E60" s="14" t="n"/>
       <c r="F60" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="61">
+    <row r="61" ht="15" customHeight="1">
       <c r="A61" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_31[c])</t>
@@ -6661,7 +6661,7 @@
       <c r="E61" s="14" t="n"/>
       <c r="F61" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="62">
+    <row r="62" ht="15" customHeight="1">
       <c r="A62" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_32[c])</t>
@@ -6683,7 +6683,7 @@
       <c r="E62" s="14" t="n"/>
       <c r="F62" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="63">
+    <row r="63" ht="15" customHeight="1">
       <c r="A63" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_33[c])</t>
@@ -6705,7 +6705,7 @@
       <c r="E63" s="14" t="n"/>
       <c r="F63" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="64">
+    <row r="64" ht="15" customHeight="1">
       <c r="A64" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_34[c])</t>
@@ -6727,7 +6727,7 @@
       <c r="E64" s="14" t="n"/>
       <c r="F64" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="65">
+    <row r="65" ht="15" customHeight="1">
       <c r="A65" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_35[c])</t>
@@ -6749,7 +6749,7 @@
       <c r="E65" s="14" t="n"/>
       <c r="F65" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="66">
+    <row r="66" ht="15" customHeight="1">
       <c r="A66" s="15" t="inlineStr">
         <is>
           <t>CONC(prot_gene_1_36[c])</t>
@@ -6771,7 +6771,7 @@
       <c r="E66" s="14" t="n"/>
       <c r="F66" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="67">
+    <row r="67" ht="15" customHeight="1">
       <c r="A67" s="15" t="inlineStr">
         <is>
           <t>CONC(ribosome[c])</t>
@@ -6793,7 +6793,7 @@
       <c r="E67" s="14" t="n"/>
       <c r="F67" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="68">
+    <row r="68" ht="15" customHeight="1">
       <c r="A68" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_1[c])</t>
@@ -6815,7 +6815,7 @@
       <c r="E68" s="14" t="n"/>
       <c r="F68" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="69">
+    <row r="69" ht="15" customHeight="1">
       <c r="A69" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_2[c])</t>
@@ -6837,7 +6837,7 @@
       <c r="E69" s="14" t="n"/>
       <c r="F69" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="70">
+    <row r="70" ht="15" customHeight="1">
       <c r="A70" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_4[c])</t>
@@ -6859,7 +6859,7 @@
       <c r="E70" s="14" t="n"/>
       <c r="F70" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="71">
+    <row r="71" ht="15" customHeight="1">
       <c r="A71" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_7[c])</t>
@@ -6881,7 +6881,7 @@
       <c r="E71" s="14" t="n"/>
       <c r="F71" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="72">
+    <row r="72" ht="15" customHeight="1">
       <c r="A72" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_8[c])</t>
@@ -6903,7 +6903,7 @@
       <c r="E72" s="14" t="n"/>
       <c r="F72" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="73">
+    <row r="73" ht="15" customHeight="1">
       <c r="A73" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_9[c])</t>
@@ -6925,7 +6925,7 @@
       <c r="E73" s="14" t="n"/>
       <c r="F73" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="74">
+    <row r="74" ht="15" customHeight="1">
       <c r="A74" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_10[c])</t>
@@ -6947,7 +6947,7 @@
       <c r="E74" s="14" t="n"/>
       <c r="F74" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="75">
+    <row r="75" ht="15" customHeight="1">
       <c r="A75" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_11[c])</t>
@@ -6969,7 +6969,7 @@
       <c r="E75" s="14" t="n"/>
       <c r="F75" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="76">
+    <row r="76" ht="15" customHeight="1">
       <c r="A76" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_12[c])</t>
@@ -6991,7 +6991,7 @@
       <c r="E76" s="14" t="n"/>
       <c r="F76" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="77">
+    <row r="77" ht="15" customHeight="1">
       <c r="A77" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_13[c])</t>
@@ -7013,7 +7013,7 @@
       <c r="E77" s="14" t="n"/>
       <c r="F77" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="78">
+    <row r="78" ht="15" customHeight="1">
       <c r="A78" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_16[c])</t>
@@ -7035,7 +7035,7 @@
       <c r="E78" s="14" t="n"/>
       <c r="F78" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="79">
+    <row r="79" ht="15" customHeight="1">
       <c r="A79" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_17[c])</t>
@@ -7057,7 +7057,7 @@
       <c r="E79" s="14" t="n"/>
       <c r="F79" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="80">
+    <row r="80" ht="15" customHeight="1">
       <c r="A80" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_18[c])</t>
@@ -7079,7 +7079,7 @@
       <c r="E80" s="14" t="n"/>
       <c r="F80" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="81">
+    <row r="81" ht="15" customHeight="1">
       <c r="A81" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_21[c])</t>
@@ -7101,7 +7101,7 @@
       <c r="E81" s="14" t="n"/>
       <c r="F81" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="82">
+    <row r="82" ht="15" customHeight="1">
       <c r="A82" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_22[c])</t>
@@ -7123,7 +7123,7 @@
       <c r="E82" s="14" t="n"/>
       <c r="F82" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="83">
+    <row r="83" ht="15" customHeight="1">
       <c r="A83" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_23[c])</t>
@@ -7145,7 +7145,7 @@
       <c r="E83" s="14" t="n"/>
       <c r="F83" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="84">
+    <row r="84" ht="15" customHeight="1">
       <c r="A84" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_24[c])</t>
@@ -7167,7 +7167,7 @@
       <c r="E84" s="14" t="n"/>
       <c r="F84" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="85">
+    <row r="85" ht="15" customHeight="1">
       <c r="A85" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_25[c])</t>
@@ -7189,7 +7189,7 @@
       <c r="E85" s="14" t="n"/>
       <c r="F85" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="86">
+    <row r="86" ht="15" customHeight="1">
       <c r="A86" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_26[c])</t>
@@ -7211,7 +7211,7 @@
       <c r="E86" s="14" t="n"/>
       <c r="F86" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="87">
+    <row r="87" ht="15" customHeight="1">
       <c r="A87" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_27[c])</t>
@@ -7233,7 +7233,7 @@
       <c r="E87" s="14" t="n"/>
       <c r="F87" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="88">
+    <row r="88" ht="15" customHeight="1">
       <c r="A88" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_28[c])</t>
@@ -7255,7 +7255,7 @@
       <c r="E88" s="14" t="n"/>
       <c r="F88" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="89">
+    <row r="89" ht="15" customHeight="1">
       <c r="A89" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_29[c])</t>
@@ -7277,7 +7277,7 @@
       <c r="E89" s="14" t="n"/>
       <c r="F89" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="90">
+    <row r="90" ht="15" customHeight="1">
       <c r="A90" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_30[c])</t>
@@ -7299,7 +7299,7 @@
       <c r="E90" s="14" t="n"/>
       <c r="F90" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="91">
+    <row r="91" ht="15" customHeight="1">
       <c r="A91" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_31[c])</t>
@@ -7321,7 +7321,7 @@
       <c r="E91" s="14" t="n"/>
       <c r="F91" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="92">
+    <row r="92" ht="15" customHeight="1">
       <c r="A92" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_32[c])</t>
@@ -7343,7 +7343,7 @@
       <c r="E92" s="14" t="n"/>
       <c r="F92" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="93">
+    <row r="93" ht="15" customHeight="1">
       <c r="A93" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_33[c])</t>
@@ -7365,7 +7365,7 @@
       <c r="E93" s="14" t="n"/>
       <c r="F93" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="94">
+    <row r="94" ht="15" customHeight="1">
       <c r="A94" s="15" t="inlineStr">
         <is>
           <t>CONC(rna_tu_1_34[c])</t>
@@ -7387,7 +7387,7 @@
       <c r="E94" s="14" t="n"/>
       <c r="F94" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="95">
+    <row r="95" ht="15" customHeight="1">
       <c r="A95" s="15" t="inlineStr">
         <is>
           <t>CONC(ser[c])</t>
@@ -7409,7 +7409,7 @@
       <c r="E95" s="14" t="n"/>
       <c r="F95" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="96">
+    <row r="96" ht="15" customHeight="1">
       <c r="A96" s="15" t="inlineStr">
         <is>
           <t>CONC(thr[c])</t>
@@ -7431,7 +7431,7 @@
       <c r="E96" s="14" t="n"/>
       <c r="F96" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="97">
+    <row r="97" ht="15" customHeight="1">
       <c r="A97" s="15" t="inlineStr">
         <is>
           <t>CONC(trp[c])</t>
@@ -7453,7 +7453,7 @@
       <c r="E97" s="14" t="n"/>
       <c r="F97" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="98">
+    <row r="98" ht="15" customHeight="1">
       <c r="A98" s="15" t="inlineStr">
         <is>
           <t>CONC(tyr[c])</t>
@@ -7475,7 +7475,7 @@
       <c r="E98" s="14" t="n"/>
       <c r="F98" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="99">
+    <row r="99" ht="15" customHeight="1">
       <c r="A99" s="15" t="inlineStr">
         <is>
           <t>CONC(ump[c])</t>
@@ -7497,7 +7497,7 @@
       <c r="E99" s="14" t="n"/>
       <c r="F99" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="100">
+    <row r="100" ht="15" customHeight="1">
       <c r="A100" s="15" t="inlineStr">
         <is>
           <t>CONC(udp[c])</t>
@@ -7519,7 +7519,7 @@
       <c r="E100" s="14" t="n"/>
       <c r="F100" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="101">
+    <row r="101" ht="15" customHeight="1">
       <c r="A101" s="15" t="inlineStr">
         <is>
           <t>CONC(utp[c])</t>
@@ -7565,7 +7565,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:F101"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7578,28 +7578,28 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="F15" pane="bottomRight" sqref="F15"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="24.5703125"/>
-    <col customWidth="1" max="3" min="2" width="20.7109375"/>
-    <col customWidth="1" max="4" min="4" style="29" width="20.7109375"/>
-    <col customWidth="1" max="7" min="5" width="20.7109375"/>
+    <col width="24.5703125" customWidth="1" min="1" max="1"/>
+    <col width="20.7109375" customWidth="1" min="2" max="3"/>
+    <col width="20.7109375" customWidth="1" style="29" min="4" max="4"/>
+    <col width="20.7109375" customWidth="1" min="5" max="7"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Observable' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='Observable' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="30" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -7636,7 +7636,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="30" t="inlineStr">
         <is>
           <t>aminoacyl_synthetase_obs</t>
@@ -7661,7 +7661,7 @@
       <c r="F3" s="14" t="n"/>
       <c r="G3" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="30" t="inlineStr">
         <is>
           <t>degrade_protease_obs</t>
@@ -7686,7 +7686,7 @@
       <c r="F4" s="14" t="n"/>
       <c r="G4" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="30" t="inlineStr">
         <is>
           <t>degrade_rnase_obs</t>
@@ -7711,7 +7711,7 @@
       <c r="F5" s="14" t="n"/>
       <c r="G5" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="30" t="inlineStr">
         <is>
           <t>ribosome_obs</t>
@@ -7736,7 +7736,7 @@
       <c r="F6" s="14" t="n"/>
       <c r="G6" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="7">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="30" t="inlineStr">
         <is>
           <t>rna_polymerase_obs</t>
@@ -7761,7 +7761,7 @@
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="8">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="30" t="inlineStr">
         <is>
           <t>translation_elongation_factors_obs</t>
@@ -7786,7 +7786,7 @@
       <c r="F8" s="14" t="n"/>
       <c r="G8" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="9">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="30" t="inlineStr">
         <is>
           <t>translation_init_factors_obs</t>
@@ -7811,7 +7811,7 @@
       <c r="F9" s="14" t="n"/>
       <c r="G9" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="10">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="30" t="inlineStr">
         <is>
           <t>translation_release_factors_obs</t>
@@ -7836,7 +7836,7 @@
       <c r="F10" s="14" t="n"/>
       <c r="G10" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="11">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="30" t="inlineStr">
         <is>
           <t>tRNA_ACG_obs</t>
@@ -7861,7 +7861,7 @@
       <c r="F11" s="14" t="n"/>
       <c r="G11" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="12">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="30" t="inlineStr">
         <is>
           <t>tRNA_ATC_obs</t>
@@ -7886,7 +7886,7 @@
       <c r="F12" s="14" t="n"/>
       <c r="G12" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="13">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="30" t="inlineStr">
         <is>
           <t>tRNA_ATG_obs</t>
@@ -7938,7 +7938,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F13"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -7951,32 +7951,32 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="J17" pane="bottomRight" sqref="J17"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="15" width="21.85546875"/>
-    <col customWidth="1" max="4" min="2" style="15" width="15.7109375"/>
-    <col customWidth="1" max="5" min="5" style="15" width="32"/>
-    <col customWidth="1" max="7" min="6" style="15" width="15.7109375"/>
-    <col customWidth="1" max="9" min="8" style="24" width="15.7109375"/>
-    <col customWidth="1" max="14" min="10" style="15" width="15.7109375"/>
-    <col customWidth="1" max="15" min="15" style="15" width="9"/>
-    <col customWidth="1" max="16384" min="16" style="15" width="9"/>
+    <col width="21.85546875" customWidth="1" style="15" min="1" max="1"/>
+    <col width="15.7109375" customWidth="1" style="15" min="2" max="4"/>
+    <col width="32" customWidth="1" style="15" min="5" max="5"/>
+    <col width="15.7109375" customWidth="1" style="15" min="6" max="7"/>
+    <col width="15.7109375" customWidth="1" style="24" min="8" max="9"/>
+    <col width="15.7109375" customWidth="1" style="15" min="10" max="14"/>
+    <col width="9" customWidth="1" style="15" min="15" max="15"/>
+    <col width="9" customWidth="1" style="15" min="16" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="8">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Reaction' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='Reaction' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -8048,7 +8048,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="26" t="inlineStr">
         <is>
           <t>mock_conversion_2amp_2atp</t>
@@ -8102,7 +8102,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J3"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -8115,24 +8115,24 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="E3" pane="bottomRight" sqref="E3"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="22" width="44.28515625"/>
-    <col customWidth="1" max="8" min="3" style="16" width="15.7109375"/>
-    <col customWidth="1" max="9" min="9" style="22" width="9"/>
-    <col customWidth="1" max="16384" min="10" style="22" width="9"/>
+    <col width="44.28515625" customWidth="1" style="22" min="1" max="2"/>
+    <col width="15.7109375" customWidth="1" style="16" min="3" max="8"/>
+    <col width="9" customWidth="1" style="22" min="9" max="9"/>
+    <col width="9" customWidth="1" style="22" min="10" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="16">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="16">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='RateLaw' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='RateLaw' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
         </is>
       </c>
     </row>
@@ -8240,7 +8240,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G3"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
@@ -8259,15 +8259,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="9" min="1" style="9" width="15.7109375"/>
-    <col customWidth="1" max="10" min="10" style="9" width="9"/>
-    <col customWidth="1" max="16384" min="11" style="9" width="9"/>
+    <col width="15.7109375" customWidth="1" style="9" min="1" max="9"/>
+    <col width="9" customWidth="1" style="9" min="10" max="10"/>
+    <col width="9" customWidth="1" style="9" min="11" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="8">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Parameter' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Parameter' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
         </is>
       </c>
     </row>
@@ -8348,7 +8348,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="5">
+    <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="11" t="inlineStr">
         <is>
           <t>K_m</t>
@@ -8363,7 +8363,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="6">
+    <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="12" t="inlineStr">
         <is>
           <t>mean_doubling_time</t>
@@ -8378,7 +8378,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="7">
+    <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="12" t="inlineStr">
         <is>
           <t>cell_density</t>
@@ -8393,7 +8393,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="8">
+    <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="12" t="inlineStr">
         <is>
           <t>fraction_dry_weight</t>
@@ -8461,7 +8461,7 @@
       <c r="E16" s="15" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8479,13 +8479,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="10" min="1" style="7" width="15.7109375"/>
+    <col width="15.7109375" customWidth="1" style="7" min="1" max="10"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6">
+    <row r="1" customFormat="1" s="6">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Evidence' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Evidence' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
         </is>
       </c>
     </row>
@@ -8542,7 +8542,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8560,13 +8560,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="13" min="1" width="20.7109375"/>
+    <col width="20.7109375" customWidth="1" min="1" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Experiment' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Experiment' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
         </is>
       </c>
     </row>
@@ -8638,7 +8638,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8651,22 +8651,22 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="K11" pane="bottomRight" sqref="K11"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Cell' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='Cell' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="column"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="30" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -8678,7 +8678,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="30" t="inlineStr">
         <is>
           <t>!Name</t>
@@ -8690,7 +8690,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="30" t="inlineStr">
         <is>
           <t>!Taxon</t>
@@ -8698,7 +8698,7 @@
       </c>
       <c r="B4" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="25.5" r="5">
+    <row r="5" ht="25.5" customHeight="1">
       <c r="A5" s="30" t="inlineStr">
         <is>
           <t>!Comments</t>
@@ -8708,8 +8708,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B4"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup horizontalDpi="1200" orientation="portrait" verticalDpi="1200"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
 </file>
 
@@ -8722,21 +8722,21 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="E6" pane="bottomRight" sqref="E6"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="12" min="1" width="15.7109375"/>
+    <col width="15.7109375" customWidth="1" min="1" max="12"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="1">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Reference' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Reference' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
         </is>
       </c>
     </row>
@@ -8804,7 +8804,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B1"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -8817,25 +8817,25 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="C15" pane="bottomRight" sqref="C15"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="6" min="1" style="29" width="20.7109375"/>
+    <col width="20.7109375" customWidth="1" style="29" min="1" max="6"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Compartment' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='Compartment' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="79" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -8867,7 +8867,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="79" t="inlineStr">
         <is>
           <t>c</t>
@@ -8899,7 +8899,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E3"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
@@ -8913,27 +8913,27 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="C2" pane="bottomRight" sqref="C2"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="10" min="1" style="15" width="20.7109375"/>
-    <col customWidth="1" max="11" min="11" style="15" width="9"/>
-    <col customWidth="1" max="16384" min="12" style="15" width="9"/>
+    <col width="20.7109375" customWidth="1" style="15" min="1" max="10"/>
+    <col width="9" customWidth="1" style="15" min="11" max="11"/>
+    <col width="9" customWidth="1" style="15" min="12" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="72">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="72">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DnaSpeciesType' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='DnaSpeciesType' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="53" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -9109,7 +9109,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I2"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -9127,21 +9127,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="6" min="1" style="55" width="20.7109375"/>
-    <col customWidth="1" max="7" min="7" style="54" width="20.7109375"/>
-    <col customWidth="1" max="12" min="8" style="55" width="20.7109375"/>
-    <col customWidth="1" max="13" min="13" style="55" width="9.140625"/>
-    <col customWidth="1" max="16384" min="14" style="55" width="9.140625"/>
+    <col width="20.7109375" customWidth="1" style="55" min="1" max="6"/>
+    <col width="20.7109375" customWidth="1" style="54" min="7" max="7"/>
+    <col width="20.7109375" customWidth="1" style="55" min="8" max="12"/>
+    <col width="9.140625" customWidth="1" style="55" min="13" max="13"/>
+    <col width="9.140625" customWidth="1" style="55" min="14" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='ChromosomeFeature' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.5" r="2">
+          <t>!!ObjTables type='Data' id='ChromosomeFeature' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="65" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -9203,7 +9203,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="3">
+    <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="66" t="inlineStr">
         <is>
           <t>DnaABox01</t>
@@ -9239,7 +9239,7 @@
       <c r="K3" s="66" t="n"/>
       <c r="L3" s="66" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="4">
+    <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="66" t="inlineStr">
         <is>
           <t>DnaABox02</t>
@@ -9273,7 +9273,7 @@
       <c r="K4" s="66" t="n"/>
       <c r="L4" s="66" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="5">
+    <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="66" t="inlineStr">
         <is>
           <t>DnaABox03</t>
@@ -9307,7 +9307,7 @@
       <c r="K5" s="66" t="n"/>
       <c r="L5" s="66" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="6">
+    <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="66" t="inlineStr">
         <is>
           <t>DnaABox04</t>
@@ -9376,7 +9376,7 @@
       <c r="L7" s="66" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9389,35 +9389,35 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="C1" pane="bottomRight" sqref="C1:C1048576"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="61" width="15.7109375"/>
-    <col customWidth="1" max="2" min="2" style="15" width="15.7109375"/>
-    <col customWidth="1" max="4" min="3" style="24" width="15.7109375"/>
-    <col customWidth="1" max="6" min="5" style="15" width="15.7109375"/>
-    <col customWidth="1" max="8" min="7" style="24" width="15.7109375"/>
-    <col customWidth="1" max="9" min="9" style="15" width="15.7109375"/>
-    <col customWidth="1" max="10" min="10" style="24" width="15.7109375"/>
-    <col customWidth="1" max="13" min="11" style="15" width="15.7109375"/>
-    <col customWidth="1" max="14" min="14" style="15" width="20.7109375"/>
-    <col customWidth="1" max="15" min="15" style="15" width="9"/>
-    <col customWidth="1" max="16384" min="16" style="15" width="9"/>
+    <col width="15.7109375" customWidth="1" style="61" min="1" max="1"/>
+    <col width="15.7109375" customWidth="1" style="15" min="2" max="2"/>
+    <col width="15.7109375" customWidth="1" style="24" min="3" max="4"/>
+    <col width="15.7109375" customWidth="1" style="15" min="5" max="6"/>
+    <col width="15.7109375" customWidth="1" style="24" min="7" max="8"/>
+    <col width="15.7109375" customWidth="1" style="15" min="9" max="9"/>
+    <col width="15.7109375" customWidth="1" style="24" min="10" max="10"/>
+    <col width="15.7109375" customWidth="1" style="15" min="11" max="13"/>
+    <col width="20.7109375" customWidth="1" style="15" min="14" max="14"/>
+    <col width="9" customWidth="1" style="15" min="15" max="15"/>
+    <col width="9" customWidth="1" style="15" min="16" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="8">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='TranscriptionUnitLocus' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='TranscriptionUnitLocus' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="62" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -9484,7 +9484,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="63" t="inlineStr">
         <is>
           <t>tu_1_1</t>
@@ -9526,7 +9526,7 @@
       <c r="K3" s="14" t="n"/>
       <c r="L3" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="63" t="inlineStr">
         <is>
           <t>tu_1_2</t>
@@ -9568,7 +9568,7 @@
       <c r="K4" s="14" t="n"/>
       <c r="L4" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="63" t="inlineStr">
         <is>
           <t>tu_1_4</t>
@@ -9610,7 +9610,7 @@
       <c r="K5" s="14" t="n"/>
       <c r="L5" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="63" t="inlineStr">
         <is>
           <t>tu_1_7</t>
@@ -9652,7 +9652,7 @@
       <c r="K6" s="14" t="n"/>
       <c r="L6" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="7">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="63" t="inlineStr">
         <is>
           <t>tu_1_8</t>
@@ -9694,7 +9694,7 @@
       <c r="K7" s="14" t="n"/>
       <c r="L7" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="8">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="63" t="inlineStr">
         <is>
           <t>tu_1_9</t>
@@ -9736,7 +9736,7 @@
       <c r="K8" s="14" t="n"/>
       <c r="L8" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="9">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="63" t="inlineStr">
         <is>
           <t>tu_1_10</t>
@@ -9778,7 +9778,7 @@
       <c r="K9" s="14" t="n"/>
       <c r="L9" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="10">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="63" t="inlineStr">
         <is>
           <t>tu_1_11</t>
@@ -9820,7 +9820,7 @@
       <c r="K10" s="14" t="n"/>
       <c r="L10" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="11">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="63" t="inlineStr">
         <is>
           <t>tu_1_12</t>
@@ -9862,7 +9862,7 @@
       <c r="K11" s="14" t="n"/>
       <c r="L11" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="12">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="63" t="inlineStr">
         <is>
           <t>tu_1_13</t>
@@ -9904,7 +9904,7 @@
       <c r="K12" s="14" t="n"/>
       <c r="L12" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="13">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="63" t="inlineStr">
         <is>
           <t>tu_1_16</t>
@@ -9946,7 +9946,7 @@
       <c r="K13" s="14" t="n"/>
       <c r="L13" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="14">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="63" t="inlineStr">
         <is>
           <t>tu_1_17</t>
@@ -9988,7 +9988,7 @@
       <c r="K14" s="14" t="n"/>
       <c r="L14" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="15">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="63" t="inlineStr">
         <is>
           <t>tu_1_18</t>
@@ -10030,7 +10030,7 @@
       <c r="K15" s="14" t="n"/>
       <c r="L15" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="16">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="63" t="inlineStr">
         <is>
           <t>tu_1_21</t>
@@ -10072,7 +10072,7 @@
       <c r="K16" s="14" t="n"/>
       <c r="L16" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="17">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="63" t="inlineStr">
         <is>
           <t>tu_1_22</t>
@@ -10114,7 +10114,7 @@
       <c r="K17" s="14" t="n"/>
       <c r="L17" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="18">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="63" t="inlineStr">
         <is>
           <t>tu_1_23</t>
@@ -10156,7 +10156,7 @@
       <c r="K18" s="14" t="n"/>
       <c r="L18" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="19">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="63" t="inlineStr">
         <is>
           <t>tu_1_24</t>
@@ -10198,7 +10198,7 @@
       <c r="K19" s="14" t="n"/>
       <c r="L19" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="20">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="63" t="inlineStr">
         <is>
           <t>tu_1_25</t>
@@ -10240,7 +10240,7 @@
       <c r="K20" s="14" t="n"/>
       <c r="L20" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="21">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="63" t="inlineStr">
         <is>
           <t>tu_1_26</t>
@@ -10282,7 +10282,7 @@
       <c r="K21" s="14" t="n"/>
       <c r="L21" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="22">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="63" t="inlineStr">
         <is>
           <t>tu_1_27</t>
@@ -10324,7 +10324,7 @@
       <c r="K22" s="14" t="n"/>
       <c r="L22" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="23">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="63" t="inlineStr">
         <is>
           <t>tu_1_28</t>
@@ -10366,7 +10366,7 @@
       <c r="K23" s="14" t="n"/>
       <c r="L23" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="24">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="63" t="inlineStr">
         <is>
           <t>tu_1_29</t>
@@ -10408,7 +10408,7 @@
       <c r="K24" s="14" t="n"/>
       <c r="L24" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="25">
+    <row r="25" ht="15" customHeight="1">
       <c r="A25" s="63" t="inlineStr">
         <is>
           <t>tu_1_30</t>
@@ -10450,7 +10450,7 @@
       <c r="K25" s="14" t="n"/>
       <c r="L25" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="26">
+    <row r="26" ht="15" customHeight="1">
       <c r="A26" s="63" t="inlineStr">
         <is>
           <t>tu_1_31</t>
@@ -10492,7 +10492,7 @@
       <c r="K26" s="14" t="n"/>
       <c r="L26" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="27">
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" s="63" t="inlineStr">
         <is>
           <t>tu_1_32</t>
@@ -10534,7 +10534,7 @@
       <c r="K27" s="14" t="n"/>
       <c r="L27" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="28">
+    <row r="28" ht="15" customHeight="1">
       <c r="A28" s="63" t="inlineStr">
         <is>
           <t>tu_1_33</t>
@@ -10576,7 +10576,7 @@
       <c r="K28" s="14" t="n"/>
       <c r="L28" s="14" t="n"/>
     </row>
-    <row customHeight="1" ht="38.25" r="29">
+    <row r="29" ht="38.25" customHeight="1">
       <c r="A29" s="63" t="inlineStr">
         <is>
           <t>tu_1_34</t>
@@ -10632,8 +10632,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L28"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup horizontalDpi="1200" orientation="portrait" verticalDpi="1200"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
 </file>
 
@@ -10646,29 +10646,29 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="G2" pane="bottomRight" sqref="G2:G37"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="4" min="1" style="55" width="15.7109375"/>
-    <col customWidth="1" max="7" min="5" style="54" width="15.7109375"/>
-    <col customWidth="1" max="15" min="8" style="55" width="15.7109375"/>
-    <col customWidth="1" max="16" min="16" style="55" width="9"/>
-    <col customWidth="1" max="16384" min="17" style="55" width="9"/>
+    <col width="15.7109375" customWidth="1" style="55" min="1" max="4"/>
+    <col width="15.7109375" customWidth="1" style="54" min="5" max="7"/>
+    <col width="15.7109375" customWidth="1" style="55" min="8" max="15"/>
+    <col width="9" customWidth="1" style="55" min="16" max="16"/>
+    <col width="9" customWidth="1" style="55" min="17" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="54">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="54">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='GeneLocus' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='GeneLocus' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="56" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -10745,7 +10745,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="57" t="inlineStr">
         <is>
           <t>gene_1_1</t>
@@ -10777,7 +10777,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="57" t="inlineStr">
         <is>
           <t>gene_1_2</t>
@@ -10809,7 +10809,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="57" t="inlineStr">
         <is>
           <t>gene_1_3</t>
@@ -10841,7 +10841,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="57" t="inlineStr">
         <is>
           <t>gene_1_4</t>
@@ -10873,7 +10873,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="57" t="inlineStr">
         <is>
           <t>gene_1_5</t>
@@ -10905,7 +10905,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="57" t="inlineStr">
         <is>
           <t>gene_1_6</t>
@@ -10937,7 +10937,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="57" t="inlineStr">
         <is>
           <t>gene_1_7</t>
@@ -10969,7 +10969,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="57" t="inlineStr">
         <is>
           <t>gene_1_8</t>
@@ -11001,7 +11001,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="11">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="57" t="inlineStr">
         <is>
           <t>gene_1_9</t>
@@ -11033,7 +11033,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="57" t="inlineStr">
         <is>
           <t>gene_1_10</t>
@@ -11065,7 +11065,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="13">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="57" t="inlineStr">
         <is>
           <t>gene_1_11</t>
@@ -11097,7 +11097,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="14">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="57" t="inlineStr">
         <is>
           <t>gene_1_12</t>
@@ -11129,7 +11129,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="15">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="57" t="inlineStr">
         <is>
           <t>gene_1_13</t>
@@ -11161,7 +11161,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="16">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="57" t="inlineStr">
         <is>
           <t>gene_1_14</t>
@@ -11193,7 +11193,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="17">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="57" t="inlineStr">
         <is>
           <t>gene_1_15</t>
@@ -11225,7 +11225,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="18">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="57" t="inlineStr">
         <is>
           <t>gene_1_16</t>
@@ -11257,7 +11257,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="19">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="57" t="inlineStr">
         <is>
           <t>gene_1_17</t>
@@ -11289,7 +11289,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="57" t="inlineStr">
         <is>
           <t>gene_1_18</t>
@@ -11321,7 +11321,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="21">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="57" t="inlineStr">
         <is>
           <t>gene_1_19</t>
@@ -11353,7 +11353,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="22">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="57" t="inlineStr">
         <is>
           <t>gene_1_20</t>
@@ -11385,7 +11385,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="23">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="57" t="inlineStr">
         <is>
           <t>gene_1_21</t>
@@ -11417,7 +11417,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="24">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="57" t="inlineStr">
         <is>
           <t>gene_1_22</t>
@@ -11449,7 +11449,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25">
+    <row r="25" ht="15" customHeight="1">
       <c r="A25" s="57" t="inlineStr">
         <is>
           <t>gene_1_23</t>
@@ -11481,7 +11481,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="26">
+    <row r="26" ht="15" customHeight="1">
       <c r="A26" s="57" t="inlineStr">
         <is>
           <t>gene_1_24</t>
@@ -11513,7 +11513,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="27">
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" s="57" t="inlineStr">
         <is>
           <t>gene_1_25</t>
@@ -11545,7 +11545,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="28">
+    <row r="28" ht="15" customHeight="1">
       <c r="A28" s="57" t="inlineStr">
         <is>
           <t>gene_1_26</t>
@@ -11577,7 +11577,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="29">
+    <row r="29" ht="15" customHeight="1">
       <c r="A29" s="57" t="inlineStr">
         <is>
           <t>gene_1_27</t>
@@ -11609,7 +11609,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="30">
+    <row r="30" ht="15" customHeight="1">
       <c r="A30" s="57" t="inlineStr">
         <is>
           <t>gene_1_28</t>
@@ -11641,7 +11641,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="31">
+    <row r="31" ht="15" customHeight="1">
       <c r="A31" s="57" t="inlineStr">
         <is>
           <t>gene_1_29</t>
@@ -11673,7 +11673,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="32">
+    <row r="32" ht="15" customHeight="1">
       <c r="A32" s="57" t="inlineStr">
         <is>
           <t>gene_1_30</t>
@@ -11705,7 +11705,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="33">
+    <row r="33" ht="15" customHeight="1">
       <c r="A33" s="57" t="inlineStr">
         <is>
           <t>gene_1_31</t>
@@ -11737,7 +11737,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="34">
+    <row r="34" ht="15" customHeight="1">
       <c r="A34" s="57" t="inlineStr">
         <is>
           <t>gene_1_32</t>
@@ -11769,7 +11769,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="35">
+    <row r="35" ht="15" customHeight="1">
       <c r="A35" s="57" t="inlineStr">
         <is>
           <t>gene_1_33</t>
@@ -11801,7 +11801,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="36">
+    <row r="36" ht="15" customHeight="1">
       <c r="A36" s="57" t="inlineStr">
         <is>
           <t>gene_1_34</t>
@@ -11833,7 +11833,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="37">
+    <row r="37" ht="15" customHeight="1">
       <c r="A37" s="57" t="inlineStr">
         <is>
           <t>gene_1_35</t>
@@ -11899,7 +11899,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I37"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -11912,29 +11912,29 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="D14" pane="bottomRight" sqref="D14"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="3" min="1" style="45" width="15.7109375"/>
-    <col customWidth="1" max="6" min="4" style="9" width="15.7109375"/>
-    <col customWidth="1" max="10" min="7" style="45" width="15.7109375"/>
-    <col customWidth="1" max="11" min="11" style="45" width="9"/>
-    <col customWidth="1" max="16384" min="12" style="45" width="9"/>
+    <col width="15.7109375" customWidth="1" style="45" min="1" max="3"/>
+    <col width="15.7109375" customWidth="1" style="9" min="4" max="6"/>
+    <col width="15.7109375" customWidth="1" style="45" min="7" max="10"/>
+    <col width="9" customWidth="1" style="45" min="11" max="11"/>
+    <col width="9" customWidth="1" style="45" min="12" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="8">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='RnaSpeciesType' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='RnaSpeciesType' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -11986,7 +11986,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_1</t>
@@ -12014,7 +12014,7 @@
       <c r="I3" s="47" t="n"/>
       <c r="J3" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_2</t>
@@ -12042,7 +12042,7 @@
       <c r="I4" s="47" t="n"/>
       <c r="J4" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_4</t>
@@ -12070,7 +12070,7 @@
       <c r="I5" s="47" t="n"/>
       <c r="J5" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_7</t>
@@ -12098,7 +12098,7 @@
       <c r="I6" s="47" t="n"/>
       <c r="J6" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="7">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_8</t>
@@ -12126,7 +12126,7 @@
       <c r="I7" s="47" t="n"/>
       <c r="J7" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="8">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_9</t>
@@ -12154,7 +12154,7 @@
       <c r="I8" s="47" t="n"/>
       <c r="J8" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="9">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_10</t>
@@ -12182,7 +12182,7 @@
       <c r="I9" s="47" t="n"/>
       <c r="J9" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="10">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_11</t>
@@ -12210,7 +12210,7 @@
       <c r="I10" s="47" t="n"/>
       <c r="J10" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="11">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_12</t>
@@ -12238,7 +12238,7 @@
       <c r="I11" s="47" t="n"/>
       <c r="J11" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="12">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_13</t>
@@ -12266,7 +12266,7 @@
       <c r="I12" s="47" t="n"/>
       <c r="J12" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="13">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_16</t>
@@ -12294,7 +12294,7 @@
       <c r="I13" s="47" t="n"/>
       <c r="J13" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="14">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_17</t>
@@ -12322,7 +12322,7 @@
       <c r="I14" s="47" t="n"/>
       <c r="J14" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="15">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_18</t>
@@ -12350,7 +12350,7 @@
       <c r="I15" s="47" t="n"/>
       <c r="J15" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="16">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_21</t>
@@ -12378,7 +12378,7 @@
       <c r="I16" s="47" t="n"/>
       <c r="J16" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="17">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_22</t>
@@ -12406,7 +12406,7 @@
       <c r="I17" s="47" t="n"/>
       <c r="J17" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="18">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_23</t>
@@ -12434,7 +12434,7 @@
       <c r="I18" s="47" t="n"/>
       <c r="J18" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="19">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_24</t>
@@ -12462,7 +12462,7 @@
       <c r="I19" s="47" t="n"/>
       <c r="J19" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="20">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_25</t>
@@ -12490,7 +12490,7 @@
       <c r="I20" s="47" t="n"/>
       <c r="J20" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="21">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_26</t>
@@ -12518,7 +12518,7 @@
       <c r="I21" s="47" t="n"/>
       <c r="J21" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="22">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_27</t>
@@ -12546,7 +12546,7 @@
       <c r="I22" s="47" t="n"/>
       <c r="J22" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="23">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_28</t>
@@ -12574,7 +12574,7 @@
       <c r="I23" s="47" t="n"/>
       <c r="J23" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="24">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_29</t>
@@ -12602,7 +12602,7 @@
       <c r="I24" s="47" t="n"/>
       <c r="J24" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="25">
+    <row r="25" ht="15" customHeight="1">
       <c r="A25" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_30</t>
@@ -12630,7 +12630,7 @@
       <c r="I25" s="47" t="n"/>
       <c r="J25" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="26">
+    <row r="26" ht="15" customHeight="1">
       <c r="A26" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_31</t>
@@ -12658,7 +12658,7 @@
       <c r="I26" s="47" t="n"/>
       <c r="J26" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="27">
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_32</t>
@@ -12686,7 +12686,7 @@
       <c r="I27" s="47" t="n"/>
       <c r="J27" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="28">
+    <row r="28" ht="15" customHeight="1">
       <c r="A28" s="52" t="inlineStr">
         <is>
           <t>rna_tu_1_33</t>
@@ -12744,7 +12744,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J28"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -12757,27 +12757,27 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
-      <selection activeCell="K40" pane="bottomRight" sqref="K40"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="7" min="1" style="45" width="15.7109375"/>
-    <col customWidth="1" max="8" min="8" style="45" width="9"/>
-    <col customWidth="1" max="16384" min="9" style="45" width="9"/>
+    <col width="15.7109375" customWidth="1" style="45" min="1" max="7"/>
+    <col width="9" customWidth="1" style="45" min="8" max="8"/>
+    <col width="9" customWidth="1" style="45" min="9" max="16384"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="8">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='ProteinSpeciesType' ObjTablesVersion='0.0.8'</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="2">
+          <t>!!ObjTables type='Data' id='ProteinSpeciesType' objTablesVersion='0.0.8' schema='wc_kb.prokaryote' tableFormat="row"</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
           <t>!Id</t>
@@ -12814,7 +12814,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_1</t>
@@ -12831,7 +12831,7 @@
       <c r="F3" s="47" t="n"/>
       <c r="G3" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_2</t>
@@ -12848,7 +12848,7 @@
       <c r="F4" s="47" t="n"/>
       <c r="G4" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_3</t>
@@ -12865,7 +12865,7 @@
       <c r="F5" s="47" t="n"/>
       <c r="G5" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="6">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_4</t>
@@ -12882,7 +12882,7 @@
       <c r="F6" s="47" t="n"/>
       <c r="G6" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="7">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_5</t>
@@ -12899,7 +12899,7 @@
       <c r="F7" s="47" t="n"/>
       <c r="G7" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="8">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_6</t>
@@ -12916,7 +12916,7 @@
       <c r="F8" s="47" t="n"/>
       <c r="G8" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="9">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_7</t>
@@ -12933,7 +12933,7 @@
       <c r="F9" s="47" t="n"/>
       <c r="G9" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="10">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_8</t>
@@ -12950,7 +12950,7 @@
       <c r="F10" s="47" t="n"/>
       <c r="G10" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="11">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_9</t>
@@ -12967,7 +12967,7 @@
       <c r="F11" s="47" t="n"/>
       <c r="G11" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="12">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_10</t>
@@ -12984,7 +12984,7 @@
       <c r="F12" s="47" t="n"/>
       <c r="G12" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="13">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_11</t>
@@ -13001,7 +13001,7 @@
       <c r="F13" s="47" t="n"/>
       <c r="G13" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="14">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_12</t>
@@ -13018,7 +13018,7 @@
       <c r="F14" s="47" t="n"/>
       <c r="G14" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="15">
+    <row r="15" ht="15" customHeight="1">
       <c r="A15" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_13</t>
@@ -13035,7 +13035,7 @@
       <c r="F15" s="47" t="n"/>
       <c r="G15" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="16">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_14</t>
@@ -13052,7 +13052,7 @@
       <c r="F16" s="47" t="n"/>
       <c r="G16" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="17">
+    <row r="17" ht="15" customHeight="1">
       <c r="A17" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_15</t>
@@ -13069,7 +13069,7 @@
       <c r="F17" s="47" t="n"/>
       <c r="G17" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="18">
+    <row r="18" ht="15" customHeight="1">
       <c r="A18" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_16</t>
@@ -13086,7 +13086,7 @@
       <c r="F18" s="47" t="n"/>
       <c r="G18" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="19">
+    <row r="19" ht="15" customHeight="1">
       <c r="A19" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_17</t>
@@ -13103,7 +13103,7 @@
       <c r="F19" s="47" t="n"/>
       <c r="G19" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="20">
+    <row r="20" ht="15" customHeight="1">
       <c r="A20" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_18</t>
@@ -13120,7 +13120,7 @@
       <c r="F20" s="47" t="n"/>
       <c r="G20" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="21">
+    <row r="21" ht="15" customHeight="1">
       <c r="A21" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_19</t>
@@ -13137,7 +13137,7 @@
       <c r="F21" s="47" t="n"/>
       <c r="G21" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="22">
+    <row r="22" ht="15" customHeight="1">
       <c r="A22" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_20</t>
@@ -13154,7 +13154,7 @@
       <c r="F22" s="47" t="n"/>
       <c r="G22" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="23">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_21</t>
@@ -13171,7 +13171,7 @@
       <c r="F23" s="47" t="n"/>
       <c r="G23" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="24">
+    <row r="24" ht="15" customHeight="1">
       <c r="A24" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_22</t>
@@ -13188,7 +13188,7 @@
       <c r="F24" s="47" t="n"/>
       <c r="G24" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="25">
+    <row r="25" ht="15" customHeight="1">
       <c r="A25" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_23</t>
@@ -13205,7 +13205,7 @@
       <c r="F25" s="47" t="n"/>
       <c r="G25" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="26">
+    <row r="26" ht="15" customHeight="1">
       <c r="A26" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_24</t>
@@ -13222,7 +13222,7 @@
       <c r="F26" s="47" t="n"/>
       <c r="G26" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="27">
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_25</t>
@@ -13239,7 +13239,7 @@
       <c r="F27" s="47" t="n"/>
       <c r="G27" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="28">
+    <row r="28" ht="15" customHeight="1">
       <c r="A28" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_26</t>
@@ -13256,7 +13256,7 @@
       <c r="F28" s="47" t="n"/>
       <c r="G28" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="29">
+    <row r="29" ht="15" customHeight="1">
       <c r="A29" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_27</t>
@@ -13273,7 +13273,7 @@
       <c r="F29" s="47" t="n"/>
       <c r="G29" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="30">
+    <row r="30" ht="15" customHeight="1">
       <c r="A30" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_28</t>
@@ -13290,7 +13290,7 @@
       <c r="F30" s="47" t="n"/>
       <c r="G30" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="31">
+    <row r="31" ht="15" customHeight="1">
       <c r="A31" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_29</t>
@@ -13307,7 +13307,7 @@
       <c r="F31" s="47" t="n"/>
       <c r="G31" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="32">
+    <row r="32" ht="15" customHeight="1">
       <c r="A32" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_30</t>
@@ -13324,7 +13324,7 @@
       <c r="F32" s="47" t="n"/>
       <c r="G32" s="47" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="33">
+    <row r="33" ht="15" customHeight="1">
       <c r="A33" s="51" t="inlineStr">
         <is>
           <t>prot_gene_1_31</t>
@@ -13408,6 +13408,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G37"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>